<commit_message>
finalize schedule and update hw0
</commit_message>
<xml_diff>
--- a/schedule_458.xlsx
+++ b/schedule_458.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH458\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFF2C3E-BC49-4010-8FBA-487EA9D0DBBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBD137F-6AA6-4748-BA03-E18B0E7028F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="weekly_schedule" sheetId="13" r:id="rId1"/>
-    <sheet name="points" sheetId="10" r:id="rId2"/>
+    <sheet name="topics" sheetId="13" r:id="rId1"/>
+    <sheet name="weekly_detail" sheetId="14" r:id="rId2"/>
+    <sheet name="points" sheetId="10" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
   <si>
     <t>Assignment</t>
   </si>
@@ -70,20 +71,12 @@
     <t>hw</t>
   </si>
   <si>
-    <t>Get connected to all the class materials &amp; tools</t>
-  </si>
-  <si>
     <t>Introduction</t>
   </si>
   <si>
     <t xml:space="preserve">Writing your own custom functions in R, and using them to generate simulations and sampling distributions. </t>
   </si>
   <si>
-    <t>* Write custom functions in R
-* Conduct a simulation experiment 
-* Construct a CI for a population parameter from a simulation experiment</t>
-  </si>
-  <si>
     <t>cn01-introduction</t>
   </si>
   <si>
@@ -102,9 +95,6 @@
     <t>Topic</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Read</t>
   </si>
   <si>
@@ -126,21 +116,12 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Objectives</t>
-  </si>
-  <si>
     <t>Syllabus</t>
   </si>
   <si>
     <t>Monday</t>
   </si>
   <si>
-    <t>Wed</t>
-  </si>
-  <si>
-    <t>Fri</t>
-  </si>
-  <si>
     <t>Worksheet</t>
   </si>
   <si>
@@ -148,9 +129,6 @@
   </si>
   <si>
     <t>worksheet 1</t>
-  </si>
-  <si>
-    <t>prac</t>
   </si>
   <si>
     <t>hw00-setup</t>
@@ -194,6 +172,52 @@
   </si>
   <si>
     <t>Ch 13</t>
+  </si>
+  <si>
+    <t>wk</t>
+  </si>
+  <si>
+    <t>Topics</t>
+  </si>
+  <si>
+    <t>SLO</t>
+  </si>
+  <si>
+    <t>Prepare</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Fall Break</t>
+  </si>
+  <si>
+    <t>Finals Week</t>
+  </si>
+  <si>
+    <t>Get connected to all the class materials &amp; tools  
+Write custom functions in R  
+Conduct a simulation experiment   
+Construct a CI for a population parameter from a simulation experiment</t>
+  </si>
+  <si>
+    <t>Welcome! Introduction to Simulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worksheet? </t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>wksht</t>
+  </si>
+  <si>
+    <t>Read the syllabus. 
+Complete [HW0](hw/hw00-setup.html)</t>
   </si>
 </sst>
 </file>
@@ -203,7 +227,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -285,24 +309,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="16"/>
       <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -315,8 +324,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -361,12 +389,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -409,7 +456,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -493,10 +540,9 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="77" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -567,99 +613,128 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="82" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" xfId="81" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="81" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="81" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="81" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="81" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="81" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="81" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="81" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="81" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="3" xfId="81" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="83" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="83" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="83" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="8" borderId="0" xfId="83" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="83" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="0" xfId="83" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="83" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="83" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="83" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="83" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="83" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="83" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="83" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="83" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="83" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="84" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="83" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="84" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="83" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="0" xfId="83" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="0" xfId="83" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="9" borderId="0" xfId="84" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="83" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="83" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="84" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="9" borderId="0" xfId="84" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="0" xfId="83" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="84" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="83" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="83" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="83" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="84" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="84" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="84" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="84" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="84" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="12" borderId="3" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="84" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="84" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="84" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="84" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="0" xfId="84" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="9" borderId="0" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="84" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="84" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="9" borderId="0" xfId="84" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="84" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="84" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="84" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="85">
-    <cellStyle name="Bad" xfId="83" builtinId="27"/>
+  <cellStyles count="84">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -738,7 +813,7 @@
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="Normal 2 2" xfId="84" xr:uid="{21148B8A-0835-4780-9D1A-ED4942764838}"/>
+    <cellStyle name="Normal 2 2" xfId="83" xr:uid="{21148B8A-0835-4780-9D1A-ED4942764838}"/>
     <cellStyle name="Normal 3" xfId="79" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
     <cellStyle name="Percent" xfId="82" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
@@ -1085,567 +1160,431 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{187BE8BD-950E-40F1-8D33-06884001169E}">
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="39"/>
-    <col min="2" max="2" width="7.375" style="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.75" style="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28" style="37" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="28" style="37" customWidth="1"/>
-    <col min="7" max="7" width="15.875" style="37" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5" style="39" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" style="42" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.125" style="42" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.25" style="42" customWidth="1"/>
-    <col min="12" max="12" width="10.75" style="36" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5" style="37" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4" style="37" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.875" style="37"/>
+    <col min="1" max="1" width="8.875" style="37"/>
+    <col min="2" max="2" width="7.375" style="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.75" style="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28" style="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" style="35" customWidth="1"/>
+    <col min="6" max="6" width="15.875" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5" style="37" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" style="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.125" style="40" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.25" style="40" customWidth="1"/>
+    <col min="11" max="16384" width="8.875" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="31" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="29" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="D1" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="E1" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="H1" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="N1" s="30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="32">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="30">
         <f>B2</f>
         <v>1</v>
       </c>
-      <c r="B2" s="32">
+      <c r="B2" s="30">
         <v>1</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-    </row>
-    <row r="3" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="38">
+      <c r="C2" s="31"/>
+      <c r="D2" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+    </row>
+    <row r="3" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="36">
         <f>A2+0.1</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="C3" s="40">
+      <c r="C3" s="38">
         <v>43122</v>
       </c>
-      <c r="D3" s="37" t="s">
-        <v>26</v>
+      <c r="D3" s="35" t="s">
+        <v>23</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="M3" s="36"/>
-    </row>
-    <row r="4" spans="1:16" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="38">
+      <c r="G3" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="63" x14ac:dyDescent="0.25">
+      <c r="A4" s="36">
         <f>A3+0.1</f>
         <v>1.2000000000000002</v>
       </c>
-      <c r="C4" s="40">
+      <c r="C4" s="38">
         <v>44588</v>
       </c>
-      <c r="D4" s="37" t="s">
-        <v>15</v>
+      <c r="D4" s="35" t="s">
+        <v>13</v>
       </c>
       <c r="E4" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="41"/>
-      <c r="I4" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="36"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="32">
+      <c r="G4" s="39"/>
+      <c r="H4" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="30">
         <f>B5</f>
         <v>2</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="30">
         <v>2</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="38">
+      <c r="C5" s="31"/>
+      <c r="D5" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="36">
         <f>A5+0.1</f>
         <v>2.1</v>
       </c>
-      <c r="H6" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="42"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="38">
-        <f>A6+0.1</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="37"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="32">
-        <f>B8</f>
+      <c r="G6" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="30">
+        <f>B7</f>
         <v>3</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B7" s="30">
         <v>3</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="48" t="s">
-        <v>41</v>
-      </c>
+      <c r="C7" s="31"/>
+      <c r="D7" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="32"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="36">
+        <f>A7+0.1</f>
+        <v>3.1</v>
+      </c>
+      <c r="D8" s="34"/>
       <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="38">
-        <f>A8+0.1</f>
-        <v>3.1</v>
-      </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="38">
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="30">
+        <f>B9</f>
+        <v>4</v>
+      </c>
+      <c r="B9" s="30">
+        <v>4</v>
+      </c>
+      <c r="C9" s="45"/>
+      <c r="D9" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="46"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="36">
         <f>A9+0.1</f>
-        <v>3.2</v>
-      </c>
-      <c r="G10" s="36"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="32">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F10" s="34"/>
+      <c r="G10" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+    </row>
+    <row r="11" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="41">
         <f>B11</f>
-        <v>4</v>
-      </c>
-      <c r="B11" s="32">
-        <v>4</v>
-      </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="41">
+        <v>5</v>
+      </c>
+      <c r="C11" s="42"/>
+      <c r="D11" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+    </row>
+    <row r="12" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="36">
+        <f>A11+0.1</f>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="40"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="35"/>
+    </row>
+    <row r="13" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="30">
+        <f>B13</f>
+        <v>6</v>
+      </c>
+      <c r="B13" s="30">
+        <v>6</v>
+      </c>
+      <c r="C13" s="31"/>
+      <c r="D13" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="35"/>
+    </row>
+    <row r="14" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="36">
+        <f>A13+0.1</f>
+        <v>6.1</v>
+      </c>
+      <c r="B14" s="37"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="G14" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="40"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+    </row>
+    <row r="15" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="30">
+        <f>B15</f>
+        <v>7</v>
+      </c>
+      <c r="B15" s="30">
+        <v>7</v>
+      </c>
+      <c r="C15" s="31"/>
+      <c r="D15" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+    </row>
+    <row r="16" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="36">
+        <f>A15+0.1</f>
+        <v>7.1</v>
+      </c>
+      <c r="B16" s="37"/>
+      <c r="C16" s="38"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="40"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+    </row>
+    <row r="17" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="30">
+        <f>B17</f>
+        <v>8</v>
+      </c>
+      <c r="B17" s="30">
+        <v>8</v>
+      </c>
+      <c r="C17" s="31"/>
+      <c r="D17" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+    </row>
+    <row r="18" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="36">
+        <f>A17+0.1</f>
+        <v>8.1</v>
+      </c>
+      <c r="B18" s="37"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="G18" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
+    </row>
+    <row r="19" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="30">
+        <f>B19</f>
+        <v>9</v>
+      </c>
+      <c r="B19" s="30">
+        <v>9</v>
+      </c>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="38">
-        <f>A11+0.1</f>
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="G12" s="36"/>
-      <c r="H12" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="J12" s="36"/>
-      <c r="K12" s="36"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="38">
-        <f>A12+0.1</f>
-        <v>4.1999999999999993</v>
-      </c>
-      <c r="G13" s="36"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="36"/>
-    </row>
-    <row r="14" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="43">
-        <f>B14</f>
-        <v>5</v>
-      </c>
-      <c r="B14" s="43">
-        <v>5</v>
-      </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="45"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="37"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="37"/>
-    </row>
-    <row r="15" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38">
-        <f>A14+0.1</f>
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="42"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="37"/>
-    </row>
-    <row r="16" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38">
-        <f>A15+0.1</f>
-        <v>5.1999999999999993</v>
-      </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="H16" s="51"/>
-      <c r="M16" s="37"/>
-      <c r="N16" s="37"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="37"/>
-    </row>
-    <row r="17" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32">
-        <f>B17</f>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="35"/>
+    </row>
+    <row r="20" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="36">
+        <f>A19+0.1</f>
+        <v>9.1</v>
+      </c>
+      <c r="B20" s="37"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="G20" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="K20" s="35"/>
+      <c r="L20" s="35"/>
+    </row>
+    <row r="21" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="41">
+        <f>B21</f>
+        <v>10</v>
+      </c>
+      <c r="B21" s="41">
+        <v>10</v>
+      </c>
+      <c r="C21" s="42"/>
+      <c r="D21" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="32">
-        <v>6</v>
-      </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="37"/>
-      <c r="P17" s="37"/>
-    </row>
-    <row r="18" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="38">
-        <f>A17+0.1</f>
-        <v>6.1</v>
-      </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="H18" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="I18" s="42"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="37"/>
-    </row>
-    <row r="19" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="38">
-        <f>A18+0.1</f>
-        <v>6.1999999999999993</v>
-      </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="H19" s="51"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="37"/>
-    </row>
-    <row r="20" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="32">
-        <f>B20</f>
-        <v>7</v>
-      </c>
-      <c r="B20" s="32">
-        <v>7</v>
-      </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="35"/>
-      <c r="M20" s="37"/>
-      <c r="N20" s="37"/>
-      <c r="O20" s="37"/>
-      <c r="P20" s="37"/>
-    </row>
-    <row r="21" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="38">
-        <f>A20+0.1</f>
-        <v>7.1</v>
-      </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="40"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="42"/>
-      <c r="M21" s="37"/>
-      <c r="N21" s="37"/>
-      <c r="O21" s="37"/>
-      <c r="P21" s="37"/>
-    </row>
-    <row r="22" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="38">
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="35"/>
+    </row>
+    <row r="22" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="36">
         <f>A21+0.1</f>
-        <v>7.1999999999999993</v>
-      </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="42"/>
-      <c r="M22" s="37"/>
-      <c r="N22" s="37"/>
-      <c r="O22" s="37"/>
-      <c r="P22" s="37"/>
-    </row>
-    <row r="23" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="32">
-        <f>B23</f>
-        <v>8</v>
-      </c>
-      <c r="B23" s="32">
-        <v>8</v>
-      </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="35"/>
-      <c r="M23" s="37"/>
-      <c r="N23" s="37"/>
-      <c r="O23" s="37"/>
-      <c r="P23" s="37"/>
-    </row>
-    <row r="24" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="38">
-        <f>A23+0.1</f>
-        <v>8.1</v>
-      </c>
-      <c r="B24" s="39"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="H24" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="M24" s="37"/>
-      <c r="N24" s="37"/>
-      <c r="O24" s="37"/>
-      <c r="P24" s="37"/>
-    </row>
-    <row r="25" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="32">
-        <f>B25</f>
-        <v>9</v>
-      </c>
-      <c r="B25" s="32">
-        <v>9</v>
-      </c>
-      <c r="C25" s="33"/>
-      <c r="D25" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35"/>
-      <c r="K25" s="35"/>
-      <c r="M25" s="37"/>
-      <c r="N25" s="37"/>
-      <c r="O25" s="37"/>
-      <c r="P25" s="37"/>
-    </row>
-    <row r="26" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="38">
-        <f>A25+0.1</f>
-        <v>9.1</v>
-      </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="H26" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="M26" s="37"/>
-      <c r="N26" s="37"/>
-      <c r="O26" s="37"/>
-      <c r="P26" s="37"/>
-    </row>
-    <row r="27" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="43">
-        <f>B27</f>
-        <v>10</v>
-      </c>
-      <c r="B27" s="43">
-        <v>10</v>
-      </c>
-      <c r="C27" s="44"/>
-      <c r="D27" s="45" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="46"/>
-      <c r="J27" s="46"/>
-      <c r="K27" s="46"/>
-      <c r="M27" s="37"/>
-      <c r="N27" s="37"/>
-      <c r="O27" s="37"/>
-      <c r="P27" s="37"/>
-    </row>
-    <row r="28" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="38">
-        <f>A27+0.1</f>
         <v>10.1</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
-      <c r="K28" s="42"/>
-      <c r="M28" s="37"/>
-      <c r="N28" s="37"/>
-      <c r="O28" s="37"/>
-      <c r="P28" s="37"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1654,6 +1593,403 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A9DCCA-5F35-4E05-A6A7-DCEBB10AE187}">
+  <dimension ref="A1:I30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.125" style="54" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="54" customWidth="1"/>
+    <col min="3" max="3" width="21.875" style="54" customWidth="1"/>
+    <col min="4" max="4" width="41.875" style="54" customWidth="1"/>
+    <col min="5" max="5" width="20.75" style="58" customWidth="1"/>
+    <col min="6" max="6" width="34.625" style="58" customWidth="1"/>
+    <col min="7" max="7" width="38" style="58" customWidth="1"/>
+    <col min="8" max="8" width="11.25" style="58" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="14.875" style="54"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="61">
+        <v>1</v>
+      </c>
+      <c r="B2" s="55">
+        <v>43487</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="61">
+        <v>2</v>
+      </c>
+      <c r="B3" s="55">
+        <f t="shared" ref="B3:B18" si="0">B2+7</f>
+        <v>43494</v>
+      </c>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3" s="40"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="61">
+        <v>3</v>
+      </c>
+      <c r="B4" s="55">
+        <f t="shared" si="0"/>
+        <v>43501</v>
+      </c>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4" s="34"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="61">
+        <v>4</v>
+      </c>
+      <c r="B5" s="55">
+        <f>B4+7</f>
+        <v>43508</v>
+      </c>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="61">
+        <v>5</v>
+      </c>
+      <c r="B6" s="55">
+        <f t="shared" si="0"/>
+        <v>43515</v>
+      </c>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="61">
+        <v>6</v>
+      </c>
+      <c r="B7" s="55">
+        <f t="shared" si="0"/>
+        <v>43522</v>
+      </c>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="61">
+        <v>7</v>
+      </c>
+      <c r="B8" s="55">
+        <f t="shared" si="0"/>
+        <v>43529</v>
+      </c>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="59"/>
+      <c r="B9" s="55">
+        <f t="shared" si="0"/>
+        <v>43536</v>
+      </c>
+      <c r="C9" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="60" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="59">
+        <v>8</v>
+      </c>
+      <c r="B10" s="55">
+        <f t="shared" si="0"/>
+        <v>43543</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="59">
+        <v>9</v>
+      </c>
+      <c r="B11" s="55">
+        <f t="shared" si="0"/>
+        <v>43550</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="59">
+        <v>10</v>
+      </c>
+      <c r="B12" s="55">
+        <f t="shared" si="0"/>
+        <v>43557</v>
+      </c>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="59">
+        <v>11</v>
+      </c>
+      <c r="B13" s="55">
+        <f t="shared" si="0"/>
+        <v>43564</v>
+      </c>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="56"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="59">
+        <v>12</v>
+      </c>
+      <c r="B14" s="55">
+        <f t="shared" si="0"/>
+        <v>43571</v>
+      </c>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="57"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="59">
+        <v>13</v>
+      </c>
+      <c r="B15" s="55">
+        <f t="shared" si="0"/>
+        <v>43578</v>
+      </c>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="59">
+        <v>14</v>
+      </c>
+      <c r="B16" s="55">
+        <f t="shared" si="0"/>
+        <v>43585</v>
+      </c>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="H16" s="56"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="59">
+        <v>15</v>
+      </c>
+      <c r="B17" s="55">
+        <f t="shared" si="0"/>
+        <v>43592</v>
+      </c>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="56"/>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="55">
+        <f t="shared" si="0"/>
+        <v>43599</v>
+      </c>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="56"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB861DFA-F44D-408D-9771-0C086E04E7DE}">
   <dimension ref="A1:J83"/>
   <sheetViews>
@@ -1677,7 +2013,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>0</v>
@@ -1700,13 +2036,13 @@
     </row>
     <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D2"/>
       <c r="F2" s="5" t="s">
@@ -1755,7 +2091,7 @@
       <c r="C5"/>
       <c r="D5"/>
       <c r="F5" s="17" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G5" s="18">
         <f>SUMIF($C$2:$C$74,F5,$D$2:$D$74)</f>

</xml_diff>

<commit_message>
work on syllabus, hw0 and cn01
</commit_message>
<xml_diff>
--- a/schedule_458.xlsx
+++ b/schedule_458.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11211"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH458\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/MATH458/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBD137F-6AA6-4748-BA03-E18B0E7028F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97A0536-7CEB-1D48-9663-1FFF70326713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="topics" sheetId="13" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
   <si>
     <t>Assignment</t>
   </si>
@@ -110,15 +110,9 @@
     <t>Midterm</t>
   </si>
   <si>
-    <t>Class Logistics</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Syllabus</t>
-  </si>
-  <si>
     <t>Monday</t>
   </si>
   <si>
@@ -135,13 +129,6 @@
   </si>
   <si>
     <t>hw01-handout</t>
-  </si>
-  <si>
-    <t>hw1_soln  
-wksht1_soln</t>
-  </si>
-  <si>
-    <t>Introduction to Sampling</t>
   </si>
   <si>
     <t>Concepts of Statistics</t>
@@ -207,9 +194,6 @@
     <t>Welcome! Introduction to Simulation</t>
   </si>
   <si>
-    <t xml:space="preserve">Worksheet? </t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
@@ -218,6 +202,32 @@
   <si>
     <t>Read the syllabus. 
 Complete [HW0](hw/hw00-setup.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to the class
+Motivating Example (Ch 1.1). Write a few sentence summary of the example and  include your take away message. </t>
+  </si>
+  <si>
+    <t>Finishing introduction to simulation notes</t>
+  </si>
+  <si>
+    <t>Population and Representative Samples (Ch 1.2)</t>
+  </si>
+  <si>
+    <t>The Sampling Problem</t>
+  </si>
+  <si>
+    <t>Use key terms in the sampling framework correctly</t>
+  </si>
+  <si>
+    <t>Welcome to the class.  
+Motivating example</t>
+  </si>
+  <si>
+    <t>Syllabus  Ch 1.1</t>
+  </si>
+  <si>
+    <t>Writing Functions in R</t>
   </si>
 </sst>
 </file>
@@ -542,7 +552,7 @@
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="77" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -723,9 +733,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1160,28 +1167,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{187BE8BD-950E-40F1-8D33-06884001169E}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="37"/>
-    <col min="2" max="2" width="7.375" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.75" style="38" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="37"/>
+    <col min="2" max="2" width="7.33203125" style="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" style="38" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" style="35" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28" style="35" customWidth="1"/>
-    <col min="6" max="6" width="15.875" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" style="35" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.5" style="37" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5" style="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.125" style="40" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.25" style="40" customWidth="1"/>
-    <col min="11" max="16384" width="8.875" style="35"/>
+    <col min="9" max="9" width="13.1640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.1640625" style="40" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="29" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="29" customFormat="1" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>14</v>
       </c>
@@ -1195,16 +1202,16 @@
         <v>17</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G1" s="27" t="s">
         <v>18</v>
       </c>
       <c r="H1" s="28" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I1" s="28" t="s">
         <v>9</v>
@@ -1213,7 +1220,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="30">
         <f>B2</f>
         <v>1</v>
@@ -1232,7 +1239,7 @@
       <c r="I2" s="33"/>
       <c r="J2" s="33"/>
     </row>
-    <row r="3" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="36">
         <f>A2+0.1</f>
         <v>1.1000000000000001</v>
@@ -1240,78 +1247,79 @@
       <c r="C3" s="38">
         <v>43122</v>
       </c>
-      <c r="D3" s="35" t="s">
-        <v>23</v>
+      <c r="D3" s="34" t="s">
+        <v>58</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="39" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="I3" s="40" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="63" x14ac:dyDescent="0.25">
-      <c r="A4" s="36">
-        <f>A3+0.1</f>
-        <v>1.2000000000000002</v>
-      </c>
-      <c r="C4" s="38">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="30">
+        <f>B4</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="30">
+        <v>2</v>
+      </c>
+      <c r="C4" s="31"/>
+      <c r="D4" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+    </row>
+    <row r="5" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="A5" s="36">
+        <f>A4+0.1</f>
+        <v>2.1</v>
+      </c>
+      <c r="C5" s="38">
         <v>44588</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D5" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E5" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F5" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="39"/>
-      <c r="H4" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="34" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="30">
-        <f>B5</f>
-        <v>2</v>
-      </c>
-      <c r="B5" s="30">
-        <v>2</v>
-      </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G5" s="39"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+    </row>
+    <row r="6" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="36">
-        <f>A5+0.1</f>
-        <v>2.1</v>
-      </c>
-      <c r="G6" s="37" t="s">
-        <v>41</v>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C6" s="38">
+        <v>43494</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="40" t="s">
+        <v>26</v>
       </c>
       <c r="I6" s="34"/>
       <c r="J6" s="34"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="30">
         <f>B7</f>
         <v>3</v>
@@ -1320,27 +1328,28 @@
         <v>3</v>
       </c>
       <c r="C7" s="31"/>
-      <c r="D7" s="46" t="s">
-        <v>34</v>
+      <c r="D7" s="32" t="s">
+        <v>56</v>
       </c>
       <c r="E7" s="32"/>
-      <c r="F7" s="51"/>
+      <c r="F7" s="32"/>
       <c r="G7" s="30"/>
       <c r="H7" s="33"/>
       <c r="I7" s="33"/>
       <c r="J7" s="33"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="36">
         <f>A7+0.1</f>
         <v>3.1</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G8" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="30">
         <f>B9</f>
         <v>4</v>
@@ -1348,86 +1357,80 @@
       <c r="B9" s="30">
         <v>4</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="46"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C9" s="31"/>
+      <c r="D9" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="32"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="36">
         <f>A9+0.1</f>
         <v>4.0999999999999996</v>
       </c>
-      <c r="F10" s="34"/>
-      <c r="G10" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-    </row>
-    <row r="11" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="41">
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="30">
         <f>B11</f>
         <v>5</v>
       </c>
-      <c r="B11" s="41">
+      <c r="B11" s="30">
         <v>5</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-    </row>
-    <row r="12" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="45"/>
+      <c r="D11" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="46"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="36">
         <f>A11+0.1</f>
         <v>5.0999999999999996</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="40"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-    </row>
-    <row r="13" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30">
+      <c r="F12" s="34"/>
+      <c r="G12" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+    </row>
+    <row r="13" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="41">
         <f>B13</f>
         <v>6</v>
       </c>
-      <c r="B13" s="30">
+      <c r="B13" s="41">
         <v>6</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
       <c r="K13" s="35"/>
       <c r="L13" s="35"/>
     </row>
-    <row r="14" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="36">
         <f>A13+0.1</f>
         <v>6.1</v>
@@ -1436,14 +1439,12 @@
       <c r="C14" s="38"/>
       <c r="D14" s="35"/>
       <c r="E14" s="35"/>
-      <c r="G14" s="49" t="s">
-        <v>21</v>
-      </c>
+      <c r="G14" s="49"/>
       <c r="H14" s="40"/>
       <c r="K14" s="35"/>
       <c r="L14" s="35"/>
     </row>
-    <row r="15" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="30">
         <f>B15</f>
         <v>7</v>
@@ -1453,30 +1454,34 @@
       </c>
       <c r="C15" s="31"/>
       <c r="D15" s="32" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E15" s="32"/>
       <c r="F15" s="32"/>
-      <c r="G15" s="30"/>
+      <c r="G15" s="50"/>
       <c r="H15" s="33"/>
       <c r="I15" s="33"/>
       <c r="J15" s="33"/>
       <c r="K15" s="35"/>
       <c r="L15" s="35"/>
     </row>
-    <row r="16" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="36">
         <f>A15+0.1</f>
         <v>7.1</v>
       </c>
       <c r="B16" s="37"/>
       <c r="C16" s="38"/>
-      <c r="G16" s="37"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="G16" s="49" t="s">
+        <v>21</v>
+      </c>
       <c r="H16" s="40"/>
       <c r="K16" s="35"/>
       <c r="L16" s="35"/>
     </row>
-    <row r="17" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="30">
         <f>B17</f>
         <v>8</v>
@@ -1486,7 +1491,7 @@
       </c>
       <c r="C17" s="31"/>
       <c r="D17" s="32" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
@@ -1497,22 +1502,19 @@
       <c r="K17" s="35"/>
       <c r="L17" s="35"/>
     </row>
-    <row r="18" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="36">
         <f>A17+0.1</f>
         <v>8.1</v>
       </c>
       <c r="B18" s="37"/>
       <c r="C18" s="38"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="G18" s="37" t="s">
-        <v>39</v>
-      </c>
+      <c r="G18" s="37"/>
+      <c r="H18" s="40"/>
       <c r="K18" s="35"/>
       <c r="L18" s="35"/>
     </row>
-    <row r="19" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="30">
         <f>B19</f>
         <v>9</v>
@@ -1522,7 +1524,7 @@
       </c>
       <c r="C19" s="31"/>
       <c r="D19" s="32" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
@@ -1533,7 +1535,7 @@
       <c r="K19" s="35"/>
       <c r="L19" s="35"/>
     </row>
-    <row r="20" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="36">
         <f>A19+0.1</f>
         <v>9.1</v>
@@ -1543,33 +1545,33 @@
       <c r="D20" s="35"/>
       <c r="E20" s="35"/>
       <c r="G20" s="37" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="K20" s="35"/>
       <c r="L20" s="35"/>
     </row>
-    <row r="21" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="41">
+    <row r="21" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="30">
         <f>B21</f>
         <v>10</v>
       </c>
-      <c r="B21" s="41">
+      <c r="B21" s="30">
         <v>10</v>
       </c>
-      <c r="C21" s="42"/>
-      <c r="D21" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="44"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
       <c r="K21" s="35"/>
       <c r="L21" s="35"/>
     </row>
-    <row r="22" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="36">
         <f>A21+0.1</f>
         <v>10.1</v>
@@ -1578,13 +1580,49 @@
       <c r="C22" s="38"/>
       <c r="D22" s="35"/>
       <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="40"/>
+      <c r="G22" s="37" t="s">
+        <v>39</v>
+      </c>
       <c r="K22" s="35"/>
       <c r="L22" s="35"/>
+    </row>
+    <row r="23" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="41">
+        <f>B23</f>
+        <v>11</v>
+      </c>
+      <c r="B23" s="41">
+        <v>11</v>
+      </c>
+      <c r="C23" s="42"/>
+      <c r="D23" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="35"/>
+    </row>
+    <row r="24" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="36">
+        <f>A23+0.1</f>
+        <v>11.1</v>
+      </c>
+      <c r="B24" s="37"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1596,100 +1634,108 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A9DCCA-5F35-4E05-A6A7-DCEBB10AE187}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.125" style="54" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" style="54" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="54" customWidth="1"/>
-    <col min="3" max="3" width="21.875" style="54" customWidth="1"/>
-    <col min="4" max="4" width="41.875" style="54" customWidth="1"/>
-    <col min="5" max="5" width="20.75" style="58" customWidth="1"/>
-    <col min="6" max="6" width="34.625" style="58" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" style="54" customWidth="1"/>
+    <col min="4" max="4" width="41.83203125" style="54" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="58" customWidth="1"/>
+    <col min="6" max="6" width="34.6640625" style="58" customWidth="1"/>
     <col min="7" max="7" width="38" style="58" customWidth="1"/>
-    <col min="8" max="8" width="11.25" style="58" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="14.875" style="54"/>
+    <col min="8" max="8" width="16.83203125" style="58" customWidth="1"/>
+    <col min="9" max="16384" width="14.83203125" style="54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="23" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="52" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B1" s="52" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="52" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="53" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="53" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" s="53" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" s="63" t="s">
+      <c r="I1" s="62" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="61">
+    <row r="2" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" s="59">
         <v>1</v>
       </c>
       <c r="B2" s="55">
         <v>43487</v>
       </c>
       <c r="C2" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="61" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="22" t="s">
         <v>53</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="62" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>8</v>
       </c>
       <c r="G2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="61" t="s">
         <v>54</v>
       </c>
       <c r="I2" s="34" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="61">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="59">
         <v>2</v>
       </c>
       <c r="B3" s="55">
         <f t="shared" ref="B3:B18" si="0">B2+7</f>
         <v>43494</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
+      <c r="C3" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="56" t="s">
+        <v>57</v>
+      </c>
       <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>55</v>
+      </c>
       <c r="H3"/>
       <c r="I3" s="40"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="61">
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="59">
         <v>3</v>
       </c>
       <c r="B4" s="55">
@@ -1704,8 +1750,8 @@
       <c r="H4"/>
       <c r="I4" s="34"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="61">
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="59">
         <v>4</v>
       </c>
       <c r="B5" s="55">
@@ -1719,8 +1765,8 @@
       <c r="G5"/>
       <c r="H5"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="61">
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="59">
         <v>5</v>
       </c>
       <c r="B6" s="55">
@@ -1734,8 +1780,8 @@
       <c r="G6"/>
       <c r="H6"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="61">
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="59">
         <v>6</v>
       </c>
       <c r="B7" s="55">
@@ -1749,8 +1795,8 @@
       <c r="G7"/>
       <c r="H7"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="61">
+    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="59">
         <v>7</v>
       </c>
       <c r="B8" s="55">
@@ -1764,30 +1810,30 @@
       <c r="G8"/>
       <c r="H8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="59"/>
       <c r="B9" s="55">
         <f t="shared" si="0"/>
         <v>43536</v>
       </c>
       <c r="C9" s="60" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D9" s="60"/>
       <c r="E9" s="60" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F9" s="60" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G9" s="60" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H9" s="60" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="59">
         <v>8</v>
       </c>
@@ -1796,7 +1842,7 @@
         <v>43543</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="59">
         <v>9</v>
       </c>
@@ -1805,7 +1851,7 @@
         <v>43550</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="59">
         <v>10</v>
       </c>
@@ -1820,7 +1866,7 @@
       <c r="G12" s="57"/>
       <c r="H12" s="57"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="59">
         <v>11</v>
       </c>
@@ -1835,7 +1881,7 @@
       <c r="G13" s="57"/>
       <c r="H13" s="56"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="59">
         <v>12</v>
       </c>
@@ -1848,7 +1894,7 @@
       <c r="G14" s="57"/>
       <c r="H14" s="57"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="59">
         <v>13</v>
       </c>
@@ -1863,7 +1909,7 @@
       <c r="G15" s="56"/>
       <c r="H15" s="56"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="59">
         <v>14</v>
       </c>
@@ -1877,7 +1923,7 @@
       <c r="F16" s="56"/>
       <c r="H16" s="56"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="59">
         <v>15</v>
       </c>
@@ -1892,9 +1938,9 @@
       <c r="G17" s="56"/>
       <c r="H17" s="56"/>
     </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="59" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B18" s="55">
         <f t="shared" si="0"/>
@@ -1907,31 +1953,31 @@
       <c r="G18" s="56"/>
       <c r="H18" s="56"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="E19"/>
       <c r="F19"/>
       <c r="G19"/>
       <c r="H19"/>
     </row>
-    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="E20"/>
       <c r="F20"/>
       <c r="G20"/>
       <c r="H20"/>
     </row>
-    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="E21"/>
       <c r="F21"/>
       <c r="G21"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="E22"/>
       <c r="F22"/>
       <c r="G22"/>
       <c r="H22"/>
     </row>
-    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C23" s="56"/>
       <c r="D23" s="56"/>
       <c r="E23"/>
@@ -1939,7 +1985,7 @@
       <c r="G23"/>
       <c r="H23"/>
     </row>
-    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C24" s="56"/>
       <c r="D24" s="56"/>
       <c r="E24"/>
@@ -1947,37 +1993,37 @@
       <c r="G24"/>
       <c r="H24"/>
     </row>
-    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="E25"/>
       <c r="F25"/>
       <c r="G25"/>
       <c r="H25"/>
     </row>
-    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26"/>
       <c r="H26"/>
     </row>
-    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27"/>
       <c r="H27"/>
     </row>
-    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="E28"/>
       <c r="F28"/>
       <c r="G28"/>
       <c r="H28"/>
     </row>
-    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29"/>
       <c r="H29"/>
     </row>
-    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30"/>
@@ -1997,21 +2043,21 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.25" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.875" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="8.875" style="3"/>
-    <col min="5" max="5" width="5.125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="3"/>
+    <col min="5" max="5" width="5.1640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="13.5" style="2" customWidth="1"/>
     <col min="7" max="7" width="10" style="3" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="3"/>
-    <col min="9" max="9" width="4.625" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="8.875" style="2"/>
+    <col min="8" max="8" width="8.83203125" style="3"/>
+    <col min="9" max="9" width="4.6640625" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -2034,15 +2080,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2"/>
       <c r="F2" s="5" t="s">
@@ -2057,7 +2103,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C3"/>
       <c r="D3"/>
       <c r="F3" s="8" t="s">
@@ -2072,7 +2118,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C4"/>
       <c r="D4"/>
       <c r="F4" s="11" t="s">
@@ -2087,11 +2133,11 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C5"/>
       <c r="D5"/>
       <c r="F5" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G5" s="18">
         <f>SUMIF($C$2:$C$74,F5,$D$2:$D$74)</f>
@@ -2102,7 +2148,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C6"/>
       <c r="D6"/>
       <c r="F6" s="14" t="s">
@@ -2117,7 +2163,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C7"/>
       <c r="D7"/>
       <c r="G7" s="16">
@@ -2125,218 +2171,218 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C8"/>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C9"/>
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C10"/>
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C11"/>
       <c r="D11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C12"/>
       <c r="D12"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C13"/>
       <c r="D13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C14"/>
       <c r="D14"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C15"/>
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C16"/>
       <c r="D16"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C17"/>
       <c r="D17"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C18"/>
       <c r="D18"/>
       <c r="G18" s="2"/>
       <c r="H18" s="23"/>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C19"/>
       <c r="D19"/>
       <c r="G19" s="2"/>
       <c r="H19" s="23"/>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C20"/>
       <c r="D20"/>
       <c r="G20" s="2"/>
       <c r="H20" s="23"/>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C21"/>
       <c r="D21"/>
       <c r="G21" s="2"/>
       <c r="H21" s="23"/>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C22"/>
       <c r="D22"/>
       <c r="G22" s="2"/>
       <c r="H22" s="23"/>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C23"/>
       <c r="D23"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C24"/>
       <c r="D24"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C25"/>
       <c r="D25"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C26"/>
       <c r="D26"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C27"/>
       <c r="D27"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C28"/>
       <c r="D28"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C29"/>
       <c r="D29"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C30"/>
       <c r="D30"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C31"/>
       <c r="D31"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C32"/>
       <c r="D32"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C33"/>
       <c r="D33"/>
     </row>
-    <row r="37" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B48" s="21"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B49" s="21"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B50" s="21"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B51" s="21"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B52" s="21"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="69" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B69" s="21"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
@@ -2344,13 +2390,13 @@
       <c r="H69" s="2"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B70" s="21"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B71" s="21"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
@@ -2358,7 +2404,7 @@
       <c r="H71" s="2"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B72" s="21"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
@@ -2366,7 +2412,7 @@
       <c r="H72" s="2"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B73" s="21"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
@@ -2374,7 +2420,7 @@
       <c r="H73" s="2"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B74" s="21"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
@@ -2382,7 +2428,7 @@
       <c r="H74" s="2"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B75" s="21"/>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
@@ -2390,7 +2436,7 @@
       <c r="H75" s="2"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B76" s="21"/>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
@@ -2398,7 +2444,7 @@
       <c r="H76" s="2"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B77" s="21"/>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
@@ -2406,7 +2452,7 @@
       <c r="H77" s="2"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B78" s="21"/>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
@@ -2414,31 +2460,31 @@
       <c r="H78" s="2"/>
       <c r="J78" s="2"/>
     </row>
-    <row r="79" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B79" s="21"/>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="J79" s="2"/>
     </row>
-    <row r="80" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B80" s="21"/>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
       <c r="J80" s="2"/>
     </row>
-    <row r="81" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B81" s="21"/>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
       <c r="J81" s="2"/>
     </row>
-    <row r="82" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B82" s="21"/>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
       <c r="J82" s="2"/>
     </row>
-    <row r="83" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B83" s="21"/>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>

</xml_diff>

<commit_message>
revise to add welcome slides and incorporate hackmd
</commit_message>
<xml_diff>
--- a/schedule_458.xlsx
+++ b/schedule_458.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH458\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\MATH458\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986774E5-D368-48CB-B4BA-8A97087534E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82370157-622C-49FC-A02E-45AA1AA89FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30120" yWindow="1950" windowWidth="27525" windowHeight="13950" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_detail" sheetId="14" r:id="rId1"/>
@@ -216,20 +216,12 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>[Intro to Simulation](notes/cn01-introduction.html) 
-Ch 1.1</t>
-  </si>
-  <si>
     <t>Use key terms in the sampling framework correctly
 Identify sources of bias and errors in surveys</t>
   </si>
   <si>
     <t xml:space="preserve">Introduction to the class. How is this all gonna work? 
 Motivating Example (Ch 1.1). Write a few sentence summary of the example and  include your take away message. </t>
-  </si>
-  <si>
-    <t>[Introduction to Sampling](notes/cn02-intro_sampling.html) 
-Ch 1.1</t>
   </si>
   <si>
     <t>Introduction to Sampling</t>
@@ -252,6 +244,16 @@
   <si>
     <t>Worksheet 1  
 Course notes: cn01 and cn02</t>
+  </si>
+  <si>
+    <t>[Introduction to Sampling](notes/cn02-intro_sampling.html)  
+[[HackMD notes]]([HackMD notes](https://hackmd.io/@norcalbiostat/cn02-intro_sampling))  
+Ch 1.1</t>
+  </si>
+  <si>
+    <t>[Welcome &amp; Course Overview](notes/cn00-welcome.html)  
+[Intro to Simulation](notes/cn01-introduction.html) 
+Ch 1.1</t>
   </si>
 </sst>
 </file>
@@ -1211,10 +1213,10 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="14.25" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="8.125" style="54" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="54" customWidth="1"/>
@@ -1227,7 +1229,7 @@
     <col min="10" max="16384" width="14.875" style="54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="21.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="52" t="s">
         <v>38</v>
       </c>
@@ -1259,7 +1261,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="110.25" x14ac:dyDescent="0.5">
       <c r="A2" s="59">
         <v>1</v>
       </c>
@@ -1276,10 +1278,10 @@
         <v>55</v>
       </c>
       <c r="F2" s="64" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H2" s="22" t="s">
         <v>10</v>
@@ -1288,10 +1290,10 @@
         <v>49</v>
       </c>
       <c r="J2" s="63" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="141.75" x14ac:dyDescent="0.5">
       <c r="A3" s="59">
         <v>2</v>
       </c>
@@ -1300,31 +1302,31 @@
         <v>43494</v>
       </c>
       <c r="C3" s="56" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D3" s="56" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" s="65" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F3" s="64" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="G3" t="s">
         <v>24</v>
       </c>
       <c r="H3" s="65" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I3" s="65" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="J3" s="40" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A4" s="59">
         <v>3</v>
       </c>
@@ -1341,7 +1343,7 @@
       <c r="I4"/>
       <c r="J4" s="34"/>
     </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A5" s="59">
         <v>4</v>
       </c>
@@ -1357,7 +1359,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A6" s="59">
         <v>5</v>
       </c>
@@ -1373,7 +1375,7 @@
       <c r="H6"/>
       <c r="I6"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A7" s="59">
         <v>6</v>
       </c>
@@ -1389,7 +1391,7 @@
       <c r="H7"/>
       <c r="I7"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A8" s="59">
         <v>7</v>
       </c>
@@ -1405,7 +1407,7 @@
       <c r="H8"/>
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A9" s="59"/>
       <c r="B9" s="55">
         <f t="shared" si="0"/>
@@ -1429,7 +1431,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A10" s="59">
         <v>8</v>
       </c>
@@ -1438,7 +1440,7 @@
         <v>43543</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A11" s="59">
         <v>9</v>
       </c>
@@ -1447,7 +1449,7 @@
         <v>43550</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A12" s="59">
         <v>10</v>
       </c>
@@ -1463,7 +1465,7 @@
       <c r="H12" s="57"/>
       <c r="I12" s="57"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A13" s="59">
         <v>11</v>
       </c>
@@ -1479,7 +1481,7 @@
       <c r="H13" s="57"/>
       <c r="I13" s="56"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A14" s="59">
         <v>12</v>
       </c>
@@ -1493,7 +1495,7 @@
       <c r="H14" s="57"/>
       <c r="I14" s="57"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A15" s="59">
         <v>13</v>
       </c>
@@ -1509,7 +1511,7 @@
       <c r="H15" s="56"/>
       <c r="I15" s="56"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A16" s="59">
         <v>14</v>
       </c>
@@ -1524,7 +1526,7 @@
       <c r="G16" s="56"/>
       <c r="I16" s="56"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A17" s="59">
         <v>15</v>
       </c>
@@ -1540,7 +1542,7 @@
       <c r="H17" s="56"/>
       <c r="I17" s="56"/>
     </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="28.5" x14ac:dyDescent="0.5">
       <c r="A18" s="59" t="s">
         <v>45</v>
       </c>
@@ -1556,35 +1558,35 @@
       <c r="H18" s="56"/>
       <c r="I18" s="56"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="E19"/>
       <c r="F19"/>
       <c r="G19"/>
       <c r="H19"/>
       <c r="I19"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="E20"/>
       <c r="F20"/>
       <c r="G20"/>
       <c r="H20"/>
       <c r="I20"/>
     </row>
-    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="E21"/>
       <c r="F21"/>
       <c r="G21"/>
       <c r="H21"/>
       <c r="I21"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="E22"/>
       <c r="F22"/>
       <c r="G22"/>
       <c r="H22"/>
       <c r="I22"/>
     </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="C23" s="56"/>
       <c r="D23" s="56"/>
       <c r="E23"/>
@@ -1593,7 +1595,7 @@
       <c r="H23"/>
       <c r="I23"/>
     </row>
-    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="C24" s="56"/>
       <c r="D24" s="56"/>
       <c r="E24"/>
@@ -1602,42 +1604,42 @@
       <c r="H24"/>
       <c r="I24"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="E25"/>
       <c r="F25"/>
       <c r="G25"/>
       <c r="H25"/>
       <c r="I25"/>
     </row>
-    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26"/>
       <c r="H26"/>
       <c r="I26"/>
     </row>
-    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27"/>
       <c r="H27"/>
       <c r="I27"/>
     </row>
-    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="E28"/>
       <c r="F28"/>
       <c r="G28"/>
       <c r="H28"/>
       <c r="I28"/>
     </row>
-    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29"/>
       <c r="H29"/>
       <c r="I29"/>
     </row>
-    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30"/>
@@ -1658,7 +1660,7 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="8.875" style="37"/>
     <col min="2" max="2" width="7.375" style="37" bestFit="1" customWidth="1"/>
@@ -1672,7 +1674,7 @@
     <col min="10" max="16384" width="8.875" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="29" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="29" customFormat="1" ht="21.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="24" t="s">
         <v>13</v>
       </c>
@@ -1701,7 +1703,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A2" s="30">
         <f>B2</f>
         <v>1</v>
@@ -1719,7 +1721,7 @@
       <c r="H2" s="33"/>
       <c r="I2" s="33"/>
     </row>
-    <row r="3" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A3" s="36">
         <f>A2+0.1</f>
         <v>1.1000000000000001</v>
@@ -1740,7 +1742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A4" s="30">
         <f>B4</f>
         <v>2</v>
@@ -1758,7 +1760,7 @@
       <c r="H4" s="33"/>
       <c r="I4" s="33"/>
     </row>
-    <row r="5" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="63" x14ac:dyDescent="0.5">
       <c r="A5" s="36">
         <f>A4+0.1</f>
         <v>2.1</v>
@@ -1778,7 +1780,7 @@
       <c r="G5" s="39"/>
       <c r="I5" s="34"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A6" s="36">
         <v>2.2000000000000002</v>
       </c>
@@ -1796,7 +1798,7 @@
       </c>
       <c r="I6" s="34"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A7" s="30">
         <f>B7</f>
         <v>3</v>
@@ -1814,7 +1816,7 @@
       <c r="H7" s="33"/>
       <c r="I7" s="33"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A8" s="36">
         <f>A7+0.1</f>
         <v>3.1</v>
@@ -1824,7 +1826,7 @@
       </c>
       <c r="I8" s="34"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A9" s="30">
         <f>B9</f>
         <v>4</v>
@@ -1842,7 +1844,7 @@
       <c r="H9" s="33"/>
       <c r="I9" s="33"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A10" s="36">
         <f>A9+0.1</f>
         <v>4.0999999999999996</v>
@@ -1852,7 +1854,7 @@
       <c r="F10" s="40"/>
       <c r="G10" s="40"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A11" s="30">
         <f>B11</f>
         <v>5</v>
@@ -1870,7 +1872,7 @@
       <c r="H11" s="48"/>
       <c r="I11" s="48"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A12" s="36">
         <f>A11+0.1</f>
         <v>5.0999999999999996</v>
@@ -1881,7 +1883,7 @@
       </c>
       <c r="I12" s="34"/>
     </row>
-    <row r="13" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A13" s="41">
         <f>B13</f>
         <v>6</v>
@@ -1901,7 +1903,7 @@
       <c r="J13" s="35"/>
       <c r="K13" s="35"/>
     </row>
-    <row r="14" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A14" s="36">
         <f>A13+0.1</f>
         <v>6.1</v>
@@ -1915,7 +1917,7 @@
       <c r="J14" s="35"/>
       <c r="K14" s="35"/>
     </row>
-    <row r="15" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A15" s="30">
         <f>B15</f>
         <v>7</v>
@@ -1935,7 +1937,7 @@
       <c r="J15" s="35"/>
       <c r="K15" s="35"/>
     </row>
-    <row r="16" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A16" s="36">
         <f>A15+0.1</f>
         <v>7.1</v>
@@ -1951,7 +1953,7 @@
       <c r="J16" s="35"/>
       <c r="K16" s="35"/>
     </row>
-    <row r="17" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A17" s="30">
         <f>B17</f>
         <v>8</v>
@@ -1971,7 +1973,7 @@
       <c r="J17" s="35"/>
       <c r="K17" s="35"/>
     </row>
-    <row r="18" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A18" s="36">
         <f>A17+0.1</f>
         <v>8.1</v>
@@ -1983,7 +1985,7 @@
       <c r="J18" s="35"/>
       <c r="K18" s="35"/>
     </row>
-    <row r="19" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A19" s="30">
         <f>B19</f>
         <v>9</v>
@@ -2003,7 +2005,7 @@
       <c r="J19" s="35"/>
       <c r="K19" s="35"/>
     </row>
-    <row r="20" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A20" s="36">
         <f>A19+0.1</f>
         <v>9.1</v>
@@ -2018,7 +2020,7 @@
       <c r="J20" s="35"/>
       <c r="K20" s="35"/>
     </row>
-    <row r="21" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A21" s="30">
         <f>B21</f>
         <v>10</v>
@@ -2038,7 +2040,7 @@
       <c r="J21" s="35"/>
       <c r="K21" s="35"/>
     </row>
-    <row r="22" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A22" s="36">
         <f>A21+0.1</f>
         <v>10.1</v>
@@ -2053,7 +2055,7 @@
       <c r="J22" s="35"/>
       <c r="K22" s="35"/>
     </row>
-    <row r="23" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A23" s="41">
         <f>B23</f>
         <v>11</v>
@@ -2073,7 +2075,7 @@
       <c r="J23" s="35"/>
       <c r="K23" s="35"/>
     </row>
-    <row r="24" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A24" s="36">
         <f>A23+0.1</f>
         <v>11.1</v>
@@ -2103,7 +2105,7 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="11.125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.875" style="21" bestFit="1" customWidth="1"/>
@@ -2117,7 +2119,7 @@
     <col min="10" max="16384" width="8.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -2140,7 +2142,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -2163,7 +2165,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C3"/>
       <c r="D3"/>
       <c r="F3" s="8" t="s">
@@ -2178,7 +2180,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C4"/>
       <c r="D4"/>
       <c r="F4" s="11" t="s">
@@ -2193,7 +2195,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C5"/>
       <c r="D5"/>
       <c r="F5" s="17" t="s">
@@ -2208,7 +2210,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C6"/>
       <c r="D6"/>
       <c r="F6" s="14" t="s">
@@ -2223,7 +2225,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C7"/>
       <c r="D7"/>
       <c r="G7" s="16">
@@ -2231,218 +2233,218 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
       <c r="C8"/>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C9"/>
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C10"/>
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C11"/>
       <c r="D11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C12"/>
       <c r="D12"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C13"/>
       <c r="D13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C14"/>
       <c r="D14"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C15"/>
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C16"/>
       <c r="D16"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C17"/>
       <c r="D17"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C18"/>
       <c r="D18"/>
       <c r="G18" s="2"/>
       <c r="H18" s="23"/>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C19"/>
       <c r="D19"/>
       <c r="G19" s="2"/>
       <c r="H19" s="23"/>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C20"/>
       <c r="D20"/>
       <c r="G20" s="2"/>
       <c r="H20" s="23"/>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C21"/>
       <c r="D21"/>
       <c r="G21" s="2"/>
       <c r="H21" s="23"/>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C22"/>
       <c r="D22"/>
       <c r="G22" s="2"/>
       <c r="H22" s="23"/>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C23"/>
       <c r="D23"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C24"/>
       <c r="D24"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C25"/>
       <c r="D25"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C26"/>
       <c r="D26"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C27"/>
       <c r="D27"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C28"/>
       <c r="D28"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C29"/>
       <c r="D29"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C30"/>
       <c r="D30"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C31"/>
       <c r="D31"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C32"/>
       <c r="D32"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.5">
       <c r="C33"/>
       <c r="D33"/>
     </row>
-    <row r="37" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B48" s="21"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B49" s="21"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B50" s="21"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B51" s="21"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B52" s="21"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="69" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B69" s="21"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
@@ -2450,13 +2452,13 @@
       <c r="H69" s="2"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B70" s="21"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B71" s="21"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
@@ -2464,7 +2466,7 @@
       <c r="H71" s="2"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B72" s="21"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
@@ -2472,7 +2474,7 @@
       <c r="H72" s="2"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B73" s="21"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
@@ -2480,7 +2482,7 @@
       <c r="H73" s="2"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B74" s="21"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
@@ -2488,7 +2490,7 @@
       <c r="H74" s="2"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B75" s="21"/>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
@@ -2496,7 +2498,7 @@
       <c r="H75" s="2"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B76" s="21"/>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
@@ -2504,7 +2506,7 @@
       <c r="H76" s="2"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B77" s="21"/>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
@@ -2512,7 +2514,7 @@
       <c r="H77" s="2"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B78" s="21"/>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
@@ -2520,31 +2522,31 @@
       <c r="H78" s="2"/>
       <c r="J78" s="2"/>
     </row>
-    <row r="79" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B79" s="21"/>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="J79" s="2"/>
     </row>
-    <row r="80" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B80" s="21"/>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
       <c r="J80" s="2"/>
     </row>
-    <row r="81" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B81" s="21"/>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
       <c r="J81" s="2"/>
     </row>
-    <row r="82" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B82" s="21"/>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
       <c r="J82" s="2"/>
     </row>
-    <row r="83" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B83" s="21"/>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>

</xml_diff>

<commit_message>
reorg week 1 and 2
</commit_message>
<xml_diff>
--- a/schedule_458.xlsx
+++ b/schedule_458.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\MATH458\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH458\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82370157-622C-49FC-A02E-45AA1AA89FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A320E543-0747-4F7B-ACE6-295EAD73E046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30075" yWindow="2220" windowWidth="26655" windowHeight="11325" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_detail" sheetId="14" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="68">
   <si>
     <t>Assignment</t>
   </si>
@@ -179,19 +179,10 @@
     <t>Finals Week</t>
   </si>
   <si>
-    <t>Get connected to all the class materials &amp; tools  
-Write custom functions in R  
-Conduct a simulation experiment   
-Construct a CI for a population parameter from a simulation experiment</t>
-  </si>
-  <si>
     <t>Welcome! Introduction to Simulation</t>
   </si>
   <si>
     <t>notes</t>
-  </si>
-  <si>
-    <t>Finishing introduction to simulation notes</t>
   </si>
   <si>
     <t>The Sampling Problem</t>
@@ -220,40 +211,55 @@
 Identify sources of bias and errors in surveys</t>
   </si>
   <si>
-    <t xml:space="preserve">Introduction to the class. How is this all gonna work? 
-Motivating Example (Ch 1.1). Write a few sentence summary of the example and  include your take away message. </t>
-  </si>
-  <si>
     <t>Introduction to Sampling</t>
-  </si>
-  <si>
-    <t>Read Ch 1.2-1.4, 1.6 before Wednesday</t>
-  </si>
-  <si>
-    <t>[HW0](hw/hw00-setup.html)</t>
   </si>
   <si>
     <t>Sampling and Nonsampling Errors (1.6)  
 Survey Design</t>
-  </si>
-  <si>
-    <t>Population and Representative Samples (Ch 1.2)   
-Sampling Bias (Ch 1.3)  
-Measurement Error (1.4)</t>
-  </si>
-  <si>
-    <t>Worksheet 1  
-Course notes: cn01 and cn02</t>
-  </si>
-  <si>
-    <t>[Introduction to Sampling](notes/cn02-intro_sampling.html)  
-[[HackMD notes]]([HackMD notes](https://hackmd.io/@norcalbiostat/cn02-intro_sampling))  
-Ch 1.1</t>
   </si>
   <si>
     <t>[Welcome &amp; Course Overview](notes/cn00-welcome.html)  
 [Intro to Simulation](notes/cn01-introduction.html) 
 Ch 1.1</t>
+  </si>
+  <si>
+    <t>[Introduction to Sampling](notes/cn02-intro_sampling.html)  
+[HackMD notes](https://hackmd.io/@norcalbiostat/cn02-intro_sampling)
+Ch 1.1</t>
+  </si>
+  <si>
+    <t>Get connected to all the class materials &amp; tools
+Write custom functions in R
+Conduct a simulation experiment
+Construct a CI for a population parameter from a simulation experiment</t>
+  </si>
+  <si>
+    <t>Introduction to the class. How is this all gonna work? 
+Motivating Example (Ch 1.1 + Canvas)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Writing your own custom functions in R, drawing samples and running repeated simulations. </t>
+  </si>
+  <si>
+    <t>Course notes: cn02</t>
+  </si>
+  <si>
+    <t>Foundations of Statistical Estimation</t>
+  </si>
+  <si>
+    <t>[HW0](hw/hw00-setup.html)  
+[Worksheet 1](worksheets/worksheet 1.pdf)
+Course notes: cn01</t>
+  </si>
+  <si>
+    <t>Using HackMD for collaborative notes
+Population and Representative Samples (Ch 1.2)   
+Sampling Bias (Ch 1.3)  
+Measurement Error (1.4)</t>
+  </si>
+  <si>
+    <t>Create a blank `cn02_username.qmd` or `cn02_username.rmd` notes file in your **notes** folder on your computer. 
+Read Ch 1.2-1.4, 1.6</t>
   </si>
 </sst>
 </file>
@@ -585,7 +591,7 @@
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="77" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -770,17 +776,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="12" borderId="3" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="83" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="11" fillId="12" borderId="3" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="83" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="83" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="83" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="84">
@@ -1213,23 +1222,25 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="14.25" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.125" style="54" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="54" customWidth="1"/>
     <col min="3" max="3" width="21.875" style="54" customWidth="1"/>
-    <col min="4" max="4" width="41.875" style="54" customWidth="1"/>
-    <col min="5" max="6" width="20.625" style="58" customWidth="1"/>
-    <col min="7" max="7" width="34.625" style="58" customWidth="1"/>
+    <col min="4" max="4" width="29.25" style="54" customWidth="1"/>
+    <col min="5" max="5" width="20.625" style="58" customWidth="1"/>
+    <col min="6" max="6" width="34.625" style="58" customWidth="1"/>
+    <col min="7" max="7" width="29.75" style="58" customWidth="1"/>
     <col min="8" max="8" width="38" style="58" customWidth="1"/>
     <col min="9" max="9" width="16.875" style="58" customWidth="1"/>
-    <col min="10" max="16384" width="14.875" style="54"/>
+    <col min="10" max="10" width="27.375" style="54" customWidth="1"/>
+    <col min="11" max="16384" width="14.875" style="54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="52" t="s">
         <v>38</v>
       </c>
@@ -1246,7 +1257,7 @@
         <v>41</v>
       </c>
       <c r="F1" s="53" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G1" s="53" t="s">
         <v>23</v>
@@ -1257,11 +1268,11 @@
       <c r="I1" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="62" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="110.25" x14ac:dyDescent="0.5">
+      <c r="J1" s="63" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A2" s="59">
         <v>1</v>
       </c>
@@ -1269,31 +1280,31 @@
         <v>43487</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="E2" s="61" t="s">
-        <v>55</v>
-      </c>
-      <c r="F2" s="64" t="s">
-        <v>66</v>
+        <v>53</v>
+      </c>
+      <c r="F2" s="62" t="s">
+        <v>58</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="I2" s="61" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" s="63" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="141.75" x14ac:dyDescent="0.5">
+        <v>24</v>
+      </c>
+      <c r="J2" s="64" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="126" x14ac:dyDescent="0.25">
       <c r="A3" s="59">
         <v>2</v>
       </c>
@@ -1302,31 +1313,29 @@
         <v>43494</v>
       </c>
       <c r="C3" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="G3" s="61" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="65" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" s="64" t="s">
-        <v>65</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="65" t="s">
+      <c r="I3" s="61"/>
+      <c r="J3" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="I3" s="65" t="s">
-        <v>62</v>
-      </c>
-      <c r="J3" s="40" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+    </row>
+    <row r="4" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="59">
         <v>3</v>
       </c>
@@ -1334,16 +1343,18 @@
         <f t="shared" si="0"/>
         <v>43501</v>
       </c>
-      <c r="C4" s="56"/>
+      <c r="C4" s="56" t="s">
+        <v>64</v>
+      </c>
       <c r="D4" s="56"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4" s="34"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="66"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="59">
         <v>4</v>
       </c>
@@ -1353,13 +1364,13 @@
       </c>
       <c r="C5" s="57"/>
       <c r="D5" s="57"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="59">
         <v>5</v>
       </c>
@@ -1369,13 +1380,13 @@
       </c>
       <c r="C6" s="57"/>
       <c r="D6" s="57"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="59">
         <v>6</v>
       </c>
@@ -1385,13 +1396,13 @@
       </c>
       <c r="C7" s="56"/>
       <c r="D7" s="56"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="59">
         <v>7</v>
       </c>
@@ -1401,13 +1412,13 @@
       </c>
       <c r="C8" s="56"/>
       <c r="D8" s="56"/>
-      <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="59"/>
       <c r="B9" s="55">
         <f t="shared" si="0"/>
@@ -1431,7 +1442,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="59">
         <v>8</v>
       </c>
@@ -1440,7 +1451,7 @@
         <v>43543</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="59">
         <v>9</v>
       </c>
@@ -1449,7 +1460,7 @@
         <v>43550</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="59">
         <v>10</v>
       </c>
@@ -1465,7 +1476,7 @@
       <c r="H12" s="57"/>
       <c r="I12" s="57"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="59">
         <v>11</v>
       </c>
@@ -1481,7 +1492,7 @@
       <c r="H13" s="57"/>
       <c r="I13" s="56"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="59">
         <v>12</v>
       </c>
@@ -1495,7 +1506,7 @@
       <c r="H14" s="57"/>
       <c r="I14" s="57"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="59">
         <v>13</v>
       </c>
@@ -1511,7 +1522,7 @@
       <c r="H15" s="56"/>
       <c r="I15" s="56"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="59">
         <v>14</v>
       </c>
@@ -1526,7 +1537,7 @@
       <c r="G16" s="56"/>
       <c r="I16" s="56"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="59">
         <v>15</v>
       </c>
@@ -1542,7 +1553,7 @@
       <c r="H17" s="56"/>
       <c r="I17" s="56"/>
     </row>
-    <row r="18" spans="1:9" ht="28.5" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="59" t="s">
         <v>45</v>
       </c>
@@ -1558,93 +1569,93 @@
       <c r="H18" s="56"/>
       <c r="I18" s="56"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19"/>
-      <c r="H19"/>
-      <c r="I19"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E21"/>
-      <c r="F21"/>
-      <c r="G21"/>
-      <c r="H21"/>
-      <c r="I21"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E22"/>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C23" s="56"/>
       <c r="D23" s="56"/>
-      <c r="E23"/>
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23"/>
-      <c r="I23"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C24" s="56"/>
       <c r="D24" s="56"/>
-      <c r="E24"/>
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24"/>
-      <c r="I24"/>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E25"/>
-      <c r="F25"/>
-      <c r="G25"/>
-      <c r="H25"/>
-      <c r="I25"/>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E26"/>
-      <c r="F26"/>
-      <c r="G26"/>
-      <c r="H26"/>
-      <c r="I26"/>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E27"/>
-      <c r="F27"/>
-      <c r="G27"/>
-      <c r="H27"/>
-      <c r="I27"/>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E28"/>
-      <c r="F28"/>
-      <c r="G28"/>
-      <c r="H28"/>
-      <c r="I28"/>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E29"/>
-      <c r="F29"/>
-      <c r="G29"/>
-      <c r="H29"/>
-      <c r="I29"/>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E30"/>
-      <c r="F30"/>
-      <c r="G30"/>
-      <c r="H30"/>
-      <c r="I30"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1660,7 +1671,7 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.875" style="37"/>
     <col min="2" max="2" width="7.375" style="37" bestFit="1" customWidth="1"/>
@@ -1674,7 +1685,7 @@
     <col min="10" max="16384" width="8.875" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="29" customFormat="1" ht="21.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" s="29" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>13</v>
       </c>
@@ -1691,19 +1702,19 @@
         <v>22</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G1" s="27" t="s">
         <v>17</v>
       </c>
       <c r="H1" s="28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I1" s="28" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="30">
         <f>B2</f>
         <v>1</v>
@@ -1721,7 +1732,7 @@
       <c r="H2" s="33"/>
       <c r="I2" s="33"/>
     </row>
-    <row r="3" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="36">
         <f>A2+0.1</f>
         <v>1.1000000000000001</v>
@@ -1730,19 +1741,19 @@
         <v>43122</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="39" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H3" s="40" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="30">
         <f>B4</f>
         <v>2</v>
@@ -1752,7 +1763,7 @@
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="32" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E4" s="32"/>
       <c r="F4" s="32"/>
@@ -1760,7 +1771,7 @@
       <c r="H4" s="33"/>
       <c r="I4" s="33"/>
     </row>
-    <row r="5" spans="1:11" ht="63" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A5" s="36">
         <f>A4+0.1</f>
         <v>2.1</v>
@@ -1780,7 +1791,7 @@
       <c r="G5" s="39"/>
       <c r="I5" s="34"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="36">
         <v>2.2000000000000002</v>
       </c>
@@ -1798,7 +1809,7 @@
       </c>
       <c r="I6" s="34"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="30">
         <f>B7</f>
         <v>3</v>
@@ -1808,7 +1819,7 @@
       </c>
       <c r="C7" s="31"/>
       <c r="D7" s="32" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E7" s="32"/>
       <c r="F7" s="32"/>
@@ -1816,7 +1827,7 @@
       <c r="H7" s="33"/>
       <c r="I7" s="33"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="36">
         <f>A7+0.1</f>
         <v>3.1</v>
@@ -1826,7 +1837,7 @@
       </c>
       <c r="I8" s="34"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="30">
         <f>B9</f>
         <v>4</v>
@@ -1844,7 +1855,7 @@
       <c r="H9" s="33"/>
       <c r="I9" s="33"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="36">
         <f>A9+0.1</f>
         <v>4.0999999999999996</v>
@@ -1854,7 +1865,7 @@
       <c r="F10" s="40"/>
       <c r="G10" s="40"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="30">
         <f>B11</f>
         <v>5</v>
@@ -1872,7 +1883,7 @@
       <c r="H11" s="48"/>
       <c r="I11" s="48"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="36">
         <f>A11+0.1</f>
         <v>5.0999999999999996</v>
@@ -1883,7 +1894,7 @@
       </c>
       <c r="I12" s="34"/>
     </row>
-    <row r="13" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="41">
         <f>B13</f>
         <v>6</v>
@@ -1903,7 +1914,7 @@
       <c r="J13" s="35"/>
       <c r="K13" s="35"/>
     </row>
-    <row r="14" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36">
         <f>A13+0.1</f>
         <v>6.1</v>
@@ -1917,7 +1928,7 @@
       <c r="J14" s="35"/>
       <c r="K14" s="35"/>
     </row>
-    <row r="15" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="30">
         <f>B15</f>
         <v>7</v>
@@ -1937,7 +1948,7 @@
       <c r="J15" s="35"/>
       <c r="K15" s="35"/>
     </row>
-    <row r="16" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36">
         <f>A15+0.1</f>
         <v>7.1</v>
@@ -1953,7 +1964,7 @@
       <c r="J16" s="35"/>
       <c r="K16" s="35"/>
     </row>
-    <row r="17" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="30">
         <f>B17</f>
         <v>8</v>
@@ -1973,7 +1984,7 @@
       <c r="J17" s="35"/>
       <c r="K17" s="35"/>
     </row>
-    <row r="18" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36">
         <f>A17+0.1</f>
         <v>8.1</v>
@@ -1985,7 +1996,7 @@
       <c r="J18" s="35"/>
       <c r="K18" s="35"/>
     </row>
-    <row r="19" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30">
         <f>B19</f>
         <v>9</v>
@@ -2005,7 +2016,7 @@
       <c r="J19" s="35"/>
       <c r="K19" s="35"/>
     </row>
-    <row r="20" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="36">
         <f>A19+0.1</f>
         <v>9.1</v>
@@ -2020,7 +2031,7 @@
       <c r="J20" s="35"/>
       <c r="K20" s="35"/>
     </row>
-    <row r="21" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="30">
         <f>B21</f>
         <v>10</v>
@@ -2040,7 +2051,7 @@
       <c r="J21" s="35"/>
       <c r="K21" s="35"/>
     </row>
-    <row r="22" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="36">
         <f>A21+0.1</f>
         <v>10.1</v>
@@ -2055,7 +2066,7 @@
       <c r="J22" s="35"/>
       <c r="K22" s="35"/>
     </row>
-    <row r="23" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="41">
         <f>B23</f>
         <v>11</v>
@@ -2075,7 +2086,7 @@
       <c r="J23" s="35"/>
       <c r="K23" s="35"/>
     </row>
-    <row r="24" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="36">
         <f>A23+0.1</f>
         <v>11.1</v>
@@ -2105,7 +2116,7 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.875" style="21" bestFit="1" customWidth="1"/>
@@ -2119,7 +2130,7 @@
     <col min="10" max="16384" width="8.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -2142,7 +2153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -2165,7 +2176,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3"/>
       <c r="D3"/>
       <c r="F3" s="8" t="s">
@@ -2180,7 +2191,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4"/>
       <c r="D4"/>
       <c r="F4" s="11" t="s">
@@ -2195,7 +2206,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5"/>
       <c r="D5"/>
       <c r="F5" s="17" t="s">
@@ -2210,7 +2221,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6"/>
       <c r="D6"/>
       <c r="F6" s="14" t="s">
@@ -2225,7 +2236,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7"/>
       <c r="D7"/>
       <c r="G7" s="16">
@@ -2233,218 +2244,218 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C8"/>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9"/>
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10"/>
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C11"/>
       <c r="D11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C12"/>
       <c r="D12"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C13"/>
       <c r="D13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14"/>
       <c r="D14"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C15"/>
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16"/>
       <c r="D16"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C17"/>
       <c r="D17"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C18"/>
       <c r="D18"/>
       <c r="G18" s="2"/>
       <c r="H18" s="23"/>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C19"/>
       <c r="D19"/>
       <c r="G19" s="2"/>
       <c r="H19" s="23"/>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C20"/>
       <c r="D20"/>
       <c r="G20" s="2"/>
       <c r="H20" s="23"/>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C21"/>
       <c r="D21"/>
       <c r="G21" s="2"/>
       <c r="H21" s="23"/>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C22"/>
       <c r="D22"/>
       <c r="G22" s="2"/>
       <c r="H22" s="23"/>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C23"/>
       <c r="D23"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C24"/>
       <c r="D24"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C25"/>
       <c r="D25"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C26"/>
       <c r="D26"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C27"/>
       <c r="D27"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C28"/>
       <c r="D28"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C29"/>
       <c r="D29"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C30"/>
       <c r="D30"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C31"/>
       <c r="D31"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C32"/>
       <c r="D32"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C33"/>
       <c r="D33"/>
     </row>
-    <row r="37" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="21"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="21"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="21"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="21"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="21"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="69" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="69" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="21"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
@@ -2452,13 +2463,13 @@
       <c r="H69" s="2"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="70" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="21"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="71" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="21"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
@@ -2466,7 +2477,7 @@
       <c r="H71" s="2"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="72" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="21"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
@@ -2474,7 +2485,7 @@
       <c r="H72" s="2"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="73" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="21"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
@@ -2482,7 +2493,7 @@
       <c r="H73" s="2"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="74" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="21"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
@@ -2490,7 +2501,7 @@
       <c r="H74" s="2"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="75" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="21"/>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
@@ -2498,7 +2509,7 @@
       <c r="H75" s="2"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="76" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="21"/>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
@@ -2506,7 +2517,7 @@
       <c r="H76" s="2"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="77" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="21"/>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
@@ -2514,7 +2525,7 @@
       <c r="H77" s="2"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="78" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="21"/>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
@@ -2522,31 +2533,31 @@
       <c r="H78" s="2"/>
       <c r="J78" s="2"/>
     </row>
-    <row r="79" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="79" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="21"/>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="J79" s="2"/>
     </row>
-    <row r="80" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="80" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="21"/>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
       <c r="J80" s="2"/>
     </row>
-    <row r="81" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="81" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B81" s="21"/>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
       <c r="J81" s="2"/>
     </row>
-    <row r="82" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="82" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B82" s="21"/>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
       <c r="J82" s="2"/>
     </row>
-    <row r="83" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="83" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B83" s="21"/>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>

</xml_diff>

<commit_message>
convert to assignments listing
</commit_message>
<xml_diff>
--- a/schedule_458.xlsx
+++ b/schedule_458.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH458\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE08092D-E8AB-4123-80C0-93F278D12A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F44428-4070-4C22-9EE7-A978CDFC4E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_detail" sheetId="14" r:id="rId1"/>
@@ -223,12 +223,6 @@
 Ch 1.1</t>
   </si>
   <si>
-    <t>Get connected to all the class materials &amp; tools
-Write custom functions in R
-Conduct a simulation experiment
-Construct a CI for a population parameter from a simulation experiment</t>
-  </si>
-  <si>
     <t>Introduction to the class. How is this all gonna work? 
 Motivating Example (Ch 1.1 + Canvas)</t>
   </si>
@@ -260,9 +254,6 @@
     <t>Properties of Estimation</t>
   </si>
   <si>
-    <t>Worksheet 2</t>
-  </si>
-  <si>
     <t>[Statistical Foundations](notes/cn03-statistical_foundations.html)  
 [HackMD notes](https://hackmd.io/@norcalbiostat/cn03-statistical_foundations)</t>
   </si>
@@ -288,6 +279,15 @@
   </si>
   <si>
     <t>No class - Robin at conference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worksheet 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get connected to all the class materials &amp; tools
+Write custom functions in R
+Conduct a simulation experiment
+</t>
   </si>
 </sst>
 </file>
@@ -1267,7 +1267,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,7 +1317,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A2" s="59">
         <v>1</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>46</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="E2" s="61" t="s">
         <v>53</v>
@@ -1337,16 +1337,16 @@
         <v>58</v>
       </c>
       <c r="G2" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="22" t="s">
-        <v>61</v>
-      </c>
       <c r="I2" s="61" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J2" s="64" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
@@ -1364,22 +1364,22 @@
         <v>55</v>
       </c>
       <c r="E3" s="61" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F3" s="62" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G3" s="61" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H3" s="61" t="s">
         <v>57</v>
       </c>
       <c r="I3" s="65" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J3" s="67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1391,28 +1391,28 @@
         <v>43501</v>
       </c>
       <c r="C4" s="56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="66" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E4" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="62" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="61" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="J4" s="64" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
rename hw files and rebulid
</commit_message>
<xml_diff>
--- a/schedule_458.xlsx
+++ b/schedule_458.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH458\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43417E74-A270-4D74-BE00-6A15EA1C831C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8486E7C7-6311-4B61-8505-4AE356236A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="77">
   <si>
     <t>Assignment</t>
   </si>
@@ -288,6 +288,11 @@
 Write custom functions in R
 Conduct a simulation experiment
 </t>
+  </si>
+  <si>
+    <t>Draw simple random samples from a data set
+Calculate estimates, errors and bounds for various parameters
+Conduct analysis using a SRS design</t>
   </si>
 </sst>
 </file>
@@ -1267,7 +1272,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1415,7 +1420,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A5" s="59">
         <v>4</v>
       </c>
@@ -1423,8 +1428,12 @@
         <f>B4+7</f>
         <v>43508</v>
       </c>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
+      <c r="C5" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="57" t="s">
+        <v>76</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>

</xml_diff>

<commit_message>
add canvas notes to cnoo
</commit_message>
<xml_diff>
--- a/schedule_458.xlsx
+++ b/schedule_458.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH458\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C6A52C-38AA-4BDA-8407-0A6D62A84BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CAE80F-1358-475D-9F7B-B9DAB57660F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32055" yWindow="1605" windowWidth="24585" windowHeight="11505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -201,9 +201,6 @@
     <t>Do</t>
   </si>
   <si>
-    <t>Look over this course website, the syllabus, and Canvas</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -256,11 +253,6 @@
 HW01</t>
   </si>
   <si>
-    <t>HW0
-Course notes: cn01
-Worksheet 1</t>
-  </si>
-  <si>
     <t>Download the `StatisticsPhD.csv` data file into your **data** folder.</t>
   </si>
   <si>
@@ -292,6 +284,17 @@
     <t>Get connected to all the class materials &amp; tools
 Write custom functions in R
 Conduct a simulation in R</t>
+  </si>
+  <si>
+    <t>Look over this course website, the syllabus, and Canvas  
+Complete the Programming Assessment  
+Download the cn01-intro_simulation_blank starter notes from Canvas before Wednesday</t>
+  </si>
+  <si>
+    <t>Programming Assessment  
+HW0
+Course notes: cn01
+Worksheet 1</t>
   </si>
 </sst>
 </file>
@@ -1269,9 +1272,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A9DCCA-5F35-4E05-A6A7-DCEBB10AE187}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1306,7 +1309,7 @@
         <v>41</v>
       </c>
       <c r="F1" s="53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G1" s="53" t="s">
         <v>23</v>
@@ -1321,7 +1324,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A2" s="59">
         <v>1</v>
       </c>
@@ -1332,25 +1335,25 @@
         <v>46</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E2" s="61" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="F2" s="62" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G2" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="22" t="s">
         <v>58</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>59</v>
       </c>
       <c r="I2" s="61" t="s">
         <v>25</v>
       </c>
       <c r="J2" s="64" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
@@ -1362,28 +1365,28 @@
         <v>43494</v>
       </c>
       <c r="C3" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="56" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="61" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" s="61" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" s="61" t="s">
-        <v>57</v>
-      </c>
       <c r="I3" s="65" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J3" s="67" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1395,28 +1398,28 @@
         <v>43501</v>
       </c>
       <c r="C4" s="56" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="62" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" s="64" t="s">
         <v>66</v>
-      </c>
-      <c r="E4" s="61" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="G4" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J4" s="64" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
@@ -1431,7 +1434,7 @@
         <v>29</v>
       </c>
       <c r="D5" s="57" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>

</xml_diff>

<commit_message>
catchup on weely overviews
</commit_message>
<xml_diff>
--- a/schedule_458.xlsx
+++ b/schedule_458.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH458\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\MATH458\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7250A0-E2F4-4BDA-931F-D76839E85527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F96F50-9760-444A-86E1-63118FF88591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_detail" sheetId="14" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="100">
   <si>
     <t>Assignment</t>
   </si>
@@ -234,10 +234,6 @@
 Measurement Error (1.4)</t>
   </si>
   <si>
-    <t>Numerical Summaries
-Variability of Estimates</t>
-  </si>
-  <si>
     <t>Properties of Estimation</t>
   </si>
   <si>
@@ -277,32 +273,112 @@
 Worksheet 1</t>
   </si>
   <si>
+    <t>[Welcome &amp; Course Overview](https://sampling-458.netlify.app/notes/cn00-welcome.html)  
+[Intro to Simulation](https://sampling-458.netlify.app/notes/cn01-intro_simulation.html)  
+Ch 1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Introduction to Sampling Framework](https://sampling-458.netlify.app/notes/cn02-intro_sampling.html)  
+[HackMD notes](https://hackmd.io/@norcalbiostat/cn02-intro_sampling)  
+Ch 1.2-1.4, 1.6  </t>
+  </si>
+  <si>
+    <t>[Statistical Foundations](https://sampling-458.netlify.app/notes/cn03-statistical_foundations.html)  
+[HackMD notes](https://hackmd.io/@norcalbiostat/cn03-statistical_foundations)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Download the `StatisticsPhD.csv` data file into your **data** folder.  
+Follow the instructions for the cn03 in Canvas. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Differentiate between a statistic and parameter
 Calculate sample statistics from data using formulas
 Estimate a population total
 Explain why estimates vary from sample to sample
-Create and describe a sampling distribution of a sample statistic
+</t>
+  </si>
+  <si>
+    <t>Create and describe a sampling distribution of a sample statistic
 Define in english and mathematically accuracy, bias and precision
-Calculate and interpret a confidence interval
-</t>
-  </si>
-  <si>
-    <t>[Welcome &amp; Course Overview](https://sampling-458.netlify.app/notes/cn00-welcome.html)  
-[Intro to Simulation](https://sampling-458.netlify.app/notes/cn01-intro_simulation.html)  
-Ch 1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Introduction to Sampling Framework](https://sampling-458.netlify.app/notes/cn02-intro_sampling.html)  
-[HackMD notes](https://hackmd.io/@norcalbiostat/cn02-intro_sampling)  
-Ch 1.2-1.4, 1.6  </t>
-  </si>
-  <si>
-    <t>[Statistical Foundations](https://sampling-458.netlify.app/notes/cn03-statistical_foundations.html)  
-[HackMD notes](https://hackmd.io/@norcalbiostat/cn03-statistical_foundations)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Download the `StatisticsPhD.csv` data file into your **data** folder.  
-Follow the instructions for the cn03 in Canvas. </t>
+Calculate and interpret a confidence interval</t>
+  </si>
+  <si>
+    <t>Worksheet 3
+Course notes: cn04
+HW02</t>
+  </si>
+  <si>
+    <t>Download ALL the datasets from the book's website. 
+Install the `sampling` and `survey` packages
+Download the cn04 blank notes template from Canvas</t>
+  </si>
+  <si>
+    <t>Worksheet 3</t>
+  </si>
+  <si>
+    <t>Variability of Estimates</t>
+  </si>
+  <si>
+    <t>Numerical Summaries</t>
+  </si>
+  <si>
+    <t>Interval Estimation</t>
+  </si>
+  <si>
+    <t>[Simple Random Sampling](https://sampling-458.netlify.app/notes/cn04-srs)</t>
+  </si>
+  <si>
+    <t>Exam 1</t>
+  </si>
+  <si>
+    <t>Drawing a SRS using multiple approaches
+Formulas for estimation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sampling weights, analysis of survey data </t>
+  </si>
+  <si>
+    <t>Strategies for learning and teaching
+Midterm Exam</t>
+  </si>
+  <si>
+    <t>Identify methods to create materials to teach others</t>
+  </si>
+  <si>
+    <t>Finalize and submit all outstanding assigments</t>
+  </si>
+  <si>
+    <t>Learning materials by teaching others</t>
+  </si>
+  <si>
+    <t>Exam review</t>
+  </si>
+  <si>
+    <t>Prepare lecture notes for stratified sampling</t>
+  </si>
+  <si>
+    <t>Stratified Sampling Methods</t>
+  </si>
+  <si>
+    <t>Draw a stratified sample from a data set
+Calculate estimates, errors and bounds for various parameters
+Conduct analysis using a stratified design</t>
+  </si>
+  <si>
+    <t>Submit lecture notes for stratified sampling to Dr D for review</t>
+  </si>
+  <si>
+    <t>Drawing a stratified sample
+Formulas for estimation</t>
+  </si>
+  <si>
+    <t>worksheet 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clean up all prior course notes to date. Check content  with classmates. </t>
+  </si>
+  <si>
+    <t>[Formulas and Definitions](https://sampling-458.netlify.app/notes/formulas.html)</t>
   </si>
 </sst>
 </file>
@@ -562,7 +638,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="84">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -647,8 +723,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="77" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -851,8 +928,11 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="84" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="84">
+  <cellStyles count="85">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -929,6 +1009,7 @@
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
     <cellStyle name="Normal 2 2" xfId="83" xr:uid="{21148B8A-0835-4780-9D1A-ED4942764838}"/>
@@ -1280,18 +1361,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A9DCCA-5F35-4E05-A6A7-DCEBB10AE187}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="14.25" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="8.125" style="54" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="54" customWidth="1"/>
     <col min="3" max="3" width="21.875" style="54" customWidth="1"/>
     <col min="4" max="4" width="29.25" style="54" customWidth="1"/>
-    <col min="5" max="5" width="20.625" style="58" customWidth="1"/>
+    <col min="5" max="5" width="30.875" style="58" customWidth="1"/>
     <col min="6" max="6" width="34.625" style="58" customWidth="1"/>
     <col min="7" max="7" width="29.75" style="58" customWidth="1"/>
     <col min="8" max="8" width="38" style="58" customWidth="1"/>
@@ -1300,7 +1381,7 @@
     <col min="11" max="16384" width="14.875" style="54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="21.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="52" t="s">
         <v>38</v>
       </c>
@@ -1332,7 +1413,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="126" x14ac:dyDescent="0.5">
       <c r="A2" s="59">
         <v>1</v>
       </c>
@@ -1343,13 +1424,13 @@
         <v>46</v>
       </c>
       <c r="D2" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="61" t="s">
-        <v>70</v>
-      </c>
       <c r="F2" s="62" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G2" s="22" t="s">
         <v>57</v>
@@ -1361,10 +1442,10 @@
         <v>25</v>
       </c>
       <c r="J2" s="64" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="126" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="126" x14ac:dyDescent="0.5">
       <c r="A3" s="59">
         <v>2</v>
       </c>
@@ -1379,10 +1460,10 @@
         <v>54</v>
       </c>
       <c r="E3" s="61" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F3" s="62" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G3" s="61" t="s">
         <v>61</v>
@@ -1391,13 +1472,13 @@
         <v>56</v>
       </c>
       <c r="I3" s="65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J3" s="66" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="114" x14ac:dyDescent="0.5">
       <c r="A4" s="59">
         <v>3</v>
       </c>
@@ -1409,28 +1490,28 @@
         <v>60</v>
       </c>
       <c r="D4" s="67" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E4" s="61" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F4" s="62" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G4" s="61" t="s">
-        <v>62</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>67</v>
+        <v>81</v>
+      </c>
+      <c r="H4" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="I4" s="61" t="s">
+        <v>80</v>
       </c>
       <c r="J4" s="64" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="76.5" x14ac:dyDescent="0.5">
       <c r="A5" s="59">
         <v>4</v>
       </c>
@@ -1438,19 +1519,29 @@
         <f>B4+7</f>
         <v>43508</v>
       </c>
-      <c r="C5" s="57" t="s">
-        <v>29</v>
+      <c r="C5" s="56" t="s">
+        <v>60</v>
       </c>
       <c r="D5" s="57" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="94.5" x14ac:dyDescent="0.5">
       <c r="A6" s="59">
         <v>5</v>
       </c>
@@ -1458,15 +1549,32 @@
         <f t="shared" si="0"/>
         <v>43515</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C6" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" s="61" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J6" s="64" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="42.75" x14ac:dyDescent="0.5">
       <c r="A7" s="59">
         <v>6</v>
       </c>
@@ -1474,15 +1582,30 @@
         <f t="shared" si="0"/>
         <v>43522</v>
       </c>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="2"/>
+      <c r="C7" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J7" s="54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="76.5" x14ac:dyDescent="0.5">
       <c r="A8" s="59">
         <v>7</v>
       </c>
@@ -1490,15 +1613,25 @@
         <f t="shared" si="0"/>
         <v>43529</v>
       </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="2"/>
+      <c r="C8" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" s="54" t="s">
+        <v>95</v>
+      </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="G8" s="61" t="s">
+        <v>96</v>
+      </c>
       <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I8" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A9" s="59"/>
       <c r="B9" s="55">
         <f t="shared" si="0"/>
@@ -1522,7 +1655,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A10" s="59">
         <v>8</v>
       </c>
@@ -1531,7 +1664,7 @@
         <v>43543</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A11" s="59">
         <v>9</v>
       </c>
@@ -1540,7 +1673,7 @@
         <v>43550</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A12" s="59">
         <v>10</v>
       </c>
@@ -1556,7 +1689,7 @@
       <c r="H12" s="57"/>
       <c r="I12" s="57"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A13" s="59">
         <v>11</v>
       </c>
@@ -1572,7 +1705,7 @@
       <c r="H13" s="57"/>
       <c r="I13" s="56"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A14" s="59">
         <v>12</v>
       </c>
@@ -1586,7 +1719,7 @@
       <c r="H14" s="57"/>
       <c r="I14" s="57"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A15" s="59">
         <v>13</v>
       </c>
@@ -1602,7 +1735,7 @@
       <c r="H15" s="56"/>
       <c r="I15" s="56"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A16" s="59">
         <v>14</v>
       </c>
@@ -1617,7 +1750,7 @@
       <c r="G16" s="56"/>
       <c r="I16" s="56"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A17" s="59">
         <v>15</v>
       </c>
@@ -1633,7 +1766,7 @@
       <c r="H17" s="56"/>
       <c r="I17" s="56"/>
     </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="28.5" x14ac:dyDescent="0.5">
       <c r="A18" s="59" t="s">
         <v>45</v>
       </c>
@@ -1649,35 +1782,35 @@
       <c r="H18" s="56"/>
       <c r="I18" s="56"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="C23" s="56"/>
       <c r="D23" s="56"/>
       <c r="E23" s="2"/>
@@ -1686,7 +1819,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="C24" s="56"/>
       <c r="D24" s="56"/>
       <c r="E24" s="2"/>
@@ -1695,42 +1828,42 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -1738,8 +1871,11 @@
       <c r="I30" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F6" r:id="rId1" display="https://sampling-458.netlify.app/notes/cn04-srs" xr:uid="{34AF491E-52E1-45F5-9C18-059B6142B2C7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1751,7 +1887,7 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="8.875" style="37"/>
     <col min="2" max="2" width="7.375" style="37" bestFit="1" customWidth="1"/>
@@ -1765,7 +1901,7 @@
     <col min="10" max="16384" width="8.875" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="29" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="29" customFormat="1" ht="21.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="24" t="s">
         <v>13</v>
       </c>
@@ -1794,7 +1930,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A2" s="30">
         <f>B2</f>
         <v>1</v>
@@ -1812,7 +1948,7 @@
       <c r="H2" s="33"/>
       <c r="I2" s="33"/>
     </row>
-    <row r="3" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A3" s="36">
         <f>A2+0.1</f>
         <v>1.1000000000000001</v>
@@ -1833,7 +1969,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A4" s="30">
         <f>B4</f>
         <v>2</v>
@@ -1851,7 +1987,7 @@
       <c r="H4" s="33"/>
       <c r="I4" s="33"/>
     </row>
-    <row r="5" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="63" x14ac:dyDescent="0.5">
       <c r="A5" s="36">
         <f>A4+0.1</f>
         <v>2.1</v>
@@ -1871,7 +2007,7 @@
       <c r="G5" s="39"/>
       <c r="I5" s="34"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A6" s="36">
         <v>2.2000000000000002</v>
       </c>
@@ -1889,7 +2025,7 @@
       </c>
       <c r="I6" s="34"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A7" s="30">
         <f>B7</f>
         <v>3</v>
@@ -1907,7 +2043,7 @@
       <c r="H7" s="33"/>
       <c r="I7" s="33"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A8" s="36">
         <f>A7+0.1</f>
         <v>3.1</v>
@@ -1917,7 +2053,7 @@
       </c>
       <c r="I8" s="34"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A9" s="30">
         <f>B9</f>
         <v>4</v>
@@ -1935,7 +2071,7 @@
       <c r="H9" s="33"/>
       <c r="I9" s="33"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A10" s="36">
         <f>A9+0.1</f>
         <v>4.0999999999999996</v>
@@ -1945,7 +2081,7 @@
       <c r="F10" s="40"/>
       <c r="G10" s="40"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A11" s="30">
         <f>B11</f>
         <v>5</v>
@@ -1963,7 +2099,7 @@
       <c r="H11" s="48"/>
       <c r="I11" s="48"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A12" s="36">
         <f>A11+0.1</f>
         <v>5.0999999999999996</v>
@@ -1974,7 +2110,7 @@
       </c>
       <c r="I12" s="34"/>
     </row>
-    <row r="13" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A13" s="41">
         <f>B13</f>
         <v>6</v>
@@ -1994,7 +2130,7 @@
       <c r="J13" s="35"/>
       <c r="K13" s="35"/>
     </row>
-    <row r="14" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A14" s="36">
         <f>A13+0.1</f>
         <v>6.1</v>
@@ -2008,7 +2144,7 @@
       <c r="J14" s="35"/>
       <c r="K14" s="35"/>
     </row>
-    <row r="15" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A15" s="30">
         <f>B15</f>
         <v>7</v>
@@ -2028,7 +2164,7 @@
       <c r="J15" s="35"/>
       <c r="K15" s="35"/>
     </row>
-    <row r="16" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A16" s="36">
         <f>A15+0.1</f>
         <v>7.1</v>
@@ -2044,7 +2180,7 @@
       <c r="J16" s="35"/>
       <c r="K16" s="35"/>
     </row>
-    <row r="17" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A17" s="30">
         <f>B17</f>
         <v>8</v>
@@ -2064,7 +2200,7 @@
       <c r="J17" s="35"/>
       <c r="K17" s="35"/>
     </row>
-    <row r="18" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A18" s="36">
         <f>A17+0.1</f>
         <v>8.1</v>
@@ -2076,7 +2212,7 @@
       <c r="J18" s="35"/>
       <c r="K18" s="35"/>
     </row>
-    <row r="19" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A19" s="30">
         <f>B19</f>
         <v>9</v>
@@ -2096,7 +2232,7 @@
       <c r="J19" s="35"/>
       <c r="K19" s="35"/>
     </row>
-    <row r="20" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A20" s="36">
         <f>A19+0.1</f>
         <v>9.1</v>
@@ -2111,7 +2247,7 @@
       <c r="J20" s="35"/>
       <c r="K20" s="35"/>
     </row>
-    <row r="21" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A21" s="30">
         <f>B21</f>
         <v>10</v>
@@ -2131,7 +2267,7 @@
       <c r="J21" s="35"/>
       <c r="K21" s="35"/>
     </row>
-    <row r="22" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A22" s="36">
         <f>A21+0.1</f>
         <v>10.1</v>
@@ -2146,7 +2282,7 @@
       <c r="J22" s="35"/>
       <c r="K22" s="35"/>
     </row>
-    <row r="23" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A23" s="41">
         <f>B23</f>
         <v>11</v>
@@ -2166,7 +2302,7 @@
       <c r="J23" s="35"/>
       <c r="K23" s="35"/>
     </row>
-    <row r="24" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A24" s="36">
         <f>A23+0.1</f>
         <v>11.1</v>
@@ -2196,7 +2332,7 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="11.125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.875" style="21" bestFit="1" customWidth="1"/>
@@ -2210,7 +2346,7 @@
     <col min="10" max="16384" width="8.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -2233,7 +2369,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -2256,7 +2392,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C3"/>
       <c r="D3"/>
       <c r="F3" s="8" t="s">
@@ -2271,7 +2407,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C4"/>
       <c r="D4"/>
       <c r="F4" s="11" t="s">
@@ -2286,7 +2422,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C5"/>
       <c r="D5"/>
       <c r="F5" s="17" t="s">
@@ -2301,7 +2437,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C6"/>
       <c r="D6"/>
       <c r="F6" s="14" t="s">
@@ -2316,7 +2452,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C7"/>
       <c r="D7"/>
       <c r="G7" s="16">
@@ -2324,218 +2460,218 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
       <c r="C8"/>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C9"/>
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C10"/>
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C11"/>
       <c r="D11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C12"/>
       <c r="D12"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C13"/>
       <c r="D13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C14"/>
       <c r="D14"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C15"/>
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
       <c r="C16"/>
       <c r="D16"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C17"/>
       <c r="D17"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C18"/>
       <c r="D18"/>
       <c r="G18" s="2"/>
       <c r="H18" s="23"/>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C19"/>
       <c r="D19"/>
       <c r="G19" s="2"/>
       <c r="H19" s="23"/>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C20"/>
       <c r="D20"/>
       <c r="G20" s="2"/>
       <c r="H20" s="23"/>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C21"/>
       <c r="D21"/>
       <c r="G21" s="2"/>
       <c r="H21" s="23"/>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C22"/>
       <c r="D22"/>
       <c r="G22" s="2"/>
       <c r="H22" s="23"/>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C23"/>
       <c r="D23"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C24"/>
       <c r="D24"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C25"/>
       <c r="D25"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C26"/>
       <c r="D26"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C27"/>
       <c r="D27"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C28"/>
       <c r="D28"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C29"/>
       <c r="D29"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C30"/>
       <c r="D30"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C31"/>
       <c r="D31"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C32"/>
       <c r="D32"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.5">
       <c r="C33"/>
       <c r="D33"/>
     </row>
-    <row r="37" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B48" s="21"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B49" s="21"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B50" s="21"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B51" s="21"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B52" s="21"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="69" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B69" s="21"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
@@ -2543,13 +2679,13 @@
       <c r="H69" s="2"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B70" s="21"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B71" s="21"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
@@ -2557,7 +2693,7 @@
       <c r="H71" s="2"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B72" s="21"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
@@ -2565,7 +2701,7 @@
       <c r="H72" s="2"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B73" s="21"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
@@ -2573,7 +2709,7 @@
       <c r="H73" s="2"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B74" s="21"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
@@ -2581,7 +2717,7 @@
       <c r="H74" s="2"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B75" s="21"/>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
@@ -2589,7 +2725,7 @@
       <c r="H75" s="2"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B76" s="21"/>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
@@ -2597,7 +2733,7 @@
       <c r="H76" s="2"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B77" s="21"/>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
@@ -2605,7 +2741,7 @@
       <c r="H77" s="2"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B78" s="21"/>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
@@ -2613,31 +2749,31 @@
       <c r="H78" s="2"/>
       <c r="J78" s="2"/>
     </row>
-    <row r="79" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B79" s="21"/>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="J79" s="2"/>
     </row>
-    <row r="80" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B80" s="21"/>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
       <c r="J80" s="2"/>
     </row>
-    <row r="81" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B81" s="21"/>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
       <c r="J81" s="2"/>
     </row>
-    <row r="82" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B82" s="21"/>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
       <c r="J82" s="2"/>
     </row>
-    <row r="83" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B83" s="21"/>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>

</xml_diff>

<commit_message>
schedule updates and add folder
</commit_message>
<xml_diff>
--- a/schedule_458.xlsx
+++ b/schedule_458.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH458\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86908FA-9636-4184-9B24-956A23F03F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8216F431-EA97-4197-B868-174F368E16BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30750" yWindow="3000" windowWidth="21600" windowHeight="11505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_detail" sheetId="14" r:id="rId1"/>
@@ -359,9 +359,6 @@
 Conduct analysis using a stratified design</t>
   </si>
   <si>
-    <t>Submit lecture notes for stratified sampling to Dr D for review</t>
-  </si>
-  <si>
     <t>Drawing a stratified sample
 Formulas for estimation</t>
   </si>
@@ -383,6 +380,10 @@
   </si>
   <si>
     <t>[Teaching and Learning](https://sampling-458.netlify.app/notes/cn05-teaching-and-learning.html)</t>
+  </si>
+  <si>
+    <t>Submit lecture notes for stratified sampling to Dr D for review
+Install the `nycflights13` package</t>
   </si>
 </sst>
 </file>
@@ -729,7 +730,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="77" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -934,6 +935,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="84" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="85">
@@ -1367,7 +1371,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1530,10 +1534,10 @@
         <v>76</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>62</v>
@@ -1563,7 +1567,7 @@
         <v>78</v>
       </c>
       <c r="F6" s="68" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G6" s="61" t="s">
         <v>84</v>
@@ -1596,13 +1600,13 @@
         <v>88</v>
       </c>
       <c r="F7" s="68" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>89</v>
       </c>
       <c r="H7" s="61" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>83</v>
@@ -1625,16 +1629,16 @@
       <c r="D8" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="E8" s="54" t="s">
-        <v>93</v>
+      <c r="E8" s="69" t="s">
+        <v>100</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="61" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add wk 8 and 9 and hackmd notes
</commit_message>
<xml_diff>
--- a/schedule_458.xlsx
+++ b/schedule_458.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH458\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8216F431-EA97-4197-B868-174F368E16BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAAC190-FF05-48F3-B6E1-A2EE4040BF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13395" yWindow="405" windowWidth="14655" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_detail" sheetId="14" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="110">
   <si>
     <t>Assignment</t>
   </si>
@@ -325,9 +325,6 @@
     <t>Interval Estimation</t>
   </si>
   <si>
-    <t>Exam 1</t>
-  </si>
-  <si>
     <t>Drawing a SRS using multiple approaches
 Formulas for estimation</t>
   </si>
@@ -348,22 +345,7 @@
     <t>Learning materials by teaching others</t>
   </si>
   <si>
-    <t>Prepare lecture notes for stratified sampling</t>
-  </si>
-  <si>
     <t>Stratified Sampling Methods</t>
-  </si>
-  <si>
-    <t>Draw a stratified sample from a data set
-Calculate estimates, errors and bounds for various parameters
-Conduct analysis using a stratified design</t>
-  </si>
-  <si>
-    <t>Drawing a stratified sample
-Formulas for estimation</t>
-  </si>
-  <si>
-    <t>worksheet 4</t>
   </si>
   <si>
     <t xml:space="preserve">Clean up all prior course notes to date. Check content  with classmates. </t>
@@ -382,8 +364,54 @@
     <t>[Teaching and Learning](https://sampling-458.netlify.app/notes/cn05-teaching-and-learning.html)</t>
   </si>
   <si>
-    <t>Submit lecture notes for stratified sampling to Dr D for review
-Install the `nycflights13` package</t>
+    <t>Exam 1 practice</t>
+  </si>
+  <si>
+    <t>Exam 1 redo</t>
+  </si>
+  <si>
+    <t>SRS Activity</t>
+  </si>
+  <si>
+    <t>Review &amp; SRS activity</t>
+  </si>
+  <si>
+    <t>Finalize ground rules for collaboration
+Exam 1 review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compare and contrast a SRS from Stratified sampling design 
+Identify correct estimates, errors and bounds for various parameters
+</t>
+  </si>
+  <si>
+    <t>Exercises</t>
+  </si>
+  <si>
+    <t>What is Stratified Sampling (Lohr 3.1)</t>
+  </si>
+  <si>
+    <t>Theory &amp; Weights (Lohr 3.2, 3.3)</t>
+  </si>
+  <si>
+    <t>Defining Strata &amp; Summary (3.5, 3.7)</t>
+  </si>
+  <si>
+    <t>Decide how to allocate observations to strata
+Practice analyzing data under a stratified random sampling framework</t>
+  </si>
+  <si>
+    <t>Review the [Ground Rules](https://canvas.csuchico.edu/courses/19460/discussion_topics/103905) discussion board in Canvas
+Read and take notes from Lohr 3.1 [using these rules](https://docs.google.com/document/d/1GzAxXqPaMIh6wGCDzcF-rYcXxlPsIAHr44Ju3VFFyw4)</t>
+  </si>
+  <si>
+    <t>Personal notes</t>
+  </si>
+  <si>
+    <t>Final group notes</t>
+  </si>
+  <si>
+    <t>Allocating Observations to Strata (3.4.1-3.4.4)</t>
   </si>
 </sst>
 </file>
@@ -1369,21 +1397,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A9DCCA-5F35-4E05-A6A7-DCEBB10AE187}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.125" style="54" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="54" customWidth="1"/>
-    <col min="3" max="3" width="21.875" style="54" customWidth="1"/>
-    <col min="4" max="4" width="29.25" style="54" customWidth="1"/>
+    <col min="3" max="3" width="19.25" style="54" customWidth="1"/>
+    <col min="4" max="4" width="25.125" style="54" customWidth="1"/>
     <col min="5" max="5" width="30.875" style="58" customWidth="1"/>
-    <col min="6" max="6" width="34.625" style="58" customWidth="1"/>
+    <col min="6" max="6" width="25.75" style="58" customWidth="1"/>
     <col min="7" max="7" width="29.75" style="58" customWidth="1"/>
-    <col min="8" max="8" width="38" style="58" customWidth="1"/>
+    <col min="8" max="8" width="30" style="58" customWidth="1"/>
     <col min="9" max="9" width="16.875" style="58" customWidth="1"/>
     <col min="10" max="10" width="27.375" style="54" customWidth="1"/>
     <col min="11" max="16384" width="14.875" style="54"/>
@@ -1421,7 +1449,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="126" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A2" s="59">
         <v>1</v>
       </c>
@@ -1453,7 +1481,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="126" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A3" s="59">
         <v>2</v>
       </c>
@@ -1486,7 +1514,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="126" x14ac:dyDescent="0.25">
       <c r="A4" s="59">
         <v>3</v>
       </c>
@@ -1519,7 +1547,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A5" s="59">
         <v>4</v>
       </c>
@@ -1534,10 +1562,10 @@
         <v>76</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>62</v>
@@ -1567,13 +1595,13 @@
         <v>78</v>
       </c>
       <c r="F6" s="68" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G6" s="61" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>79</v>
@@ -1591,31 +1619,28 @@
         <v>43522</v>
       </c>
       <c r="C7" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="56" t="s">
+      <c r="E7" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F7" s="68" t="s">
-        <v>99</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="H7" s="61" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="J7" s="54" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="59">
         <v>7</v>
       </c>
@@ -1624,21 +1649,19 @@
         <v>43529</v>
       </c>
       <c r="C8" s="56" t="s">
-        <v>91</v>
-      </c>
-      <c r="D8" s="57" t="s">
-        <v>92</v>
-      </c>
-      <c r="E8" s="69" t="s">
-        <v>100</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="D8" s="57"/>
+      <c r="E8" s="69"/>
       <c r="F8" s="2"/>
       <c r="G8" s="61" t="s">
-        <v>93</v>
-      </c>
-      <c r="H8" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="I8" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1665,7 +1688,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="59">
         <v>8</v>
       </c>
@@ -1673,14 +1696,47 @@
         <f t="shared" si="0"/>
         <v>43543</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="56" t="s">
+        <v>106</v>
+      </c>
+      <c r="G10" s="56" t="s">
+        <v>102</v>
+      </c>
+      <c r="H10" s="56" t="s">
+        <v>103</v>
+      </c>
+      <c r="I10" s="58" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="59">
         <v>9</v>
       </c>
       <c r="B11" s="55">
         <f t="shared" si="0"/>
         <v>43550</v>
+      </c>
+      <c r="C11" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="69" t="s">
+        <v>105</v>
+      </c>
+      <c r="G11" s="56" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" s="56" t="s">
+        <v>104</v>
+      </c>
+      <c r="I11" s="58" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2340,7 +2396,7 @@
   <dimension ref="A1:J83"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2508,87 +2564,97 @@
       <c r="D16"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="21" t="s">
+        <v>107</v>
+      </c>
       <c r="C17"/>
-      <c r="D17"/>
+      <c r="D17">
+        <v>2.5</v>
+      </c>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="21" t="s">
+        <v>108</v>
+      </c>
       <c r="C18"/>
-      <c r="D18"/>
+      <c r="D18">
+        <v>2.5</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="23"/>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C19"/>
       <c r="D19"/>
       <c r="G19" s="2"/>
       <c r="H19" s="23"/>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C20"/>
       <c r="D20"/>
       <c r="G20" s="2"/>
       <c r="H20" s="23"/>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C21"/>
       <c r="D21"/>
       <c r="G21" s="2"/>
       <c r="H21" s="23"/>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C22"/>
       <c r="D22"/>
       <c r="G22" s="2"/>
       <c r="H22" s="23"/>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C23"/>
       <c r="D23"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C24"/>
       <c r="D24"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C25"/>
       <c r="D25"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C26"/>
       <c r="D26"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C27"/>
       <c r="D27"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C28"/>
       <c r="D28"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C29"/>
       <c r="D29"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C30"/>
       <c r="D30"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C31"/>
       <c r="D31"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C32"/>
       <c r="D32"/>
       <c r="G32" s="2"/>

</xml_diff>

<commit_message>
dont render collab notes start cn06
</commit_message>
<xml_diff>
--- a/schedule_458.xlsx
+++ b/schedule_458.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH458\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAAC190-FF05-48F3-B6E1-A2EE4040BF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F234FA0-8B04-486D-A802-8A96CB04F3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13395" yWindow="405" windowWidth="14655" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="111">
   <si>
     <t>Assignment</t>
   </si>
@@ -412,6 +412,10 @@
   </si>
   <si>
     <t>Allocating Observations to Strata (3.4.1-3.4.4)</t>
+  </si>
+  <si>
+    <t>[Live Notes]()
+[HackMD Collab Notes](https://hackmd.io/@norcalbiostat/cn06_stratified)</t>
   </si>
 </sst>
 </file>
@@ -1399,7 +1403,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1704,6 +1708,9 @@
       </c>
       <c r="E10" s="56" t="s">
         <v>106</v>
+      </c>
+      <c r="F10" s="56" t="s">
+        <v>110</v>
       </c>
       <c r="G10" s="56" t="s">
         <v>102</v>

</xml_diff>